<commit_message>
Added CMIP6 GWLs to all OEKS15 models
</commit_message>
<xml_diff>
--- a/data/gwl_lists/GWLs_CMIP5_OEKS15.xlsx
+++ b/data/gwl_lists/GWLs_CMIP5_OEKS15.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbecsi/Desktop/Arbeit/Qgis/data/AAR2/GWLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09C9F78-E25D-1A4A-8BBB-6644662F2D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859FE6EE-AAAA-F646-8C4A-D5557ADCEF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22120" xr2:uid="{B7CF2435-4AB2-8449-A283-99C1C1B4CF66}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22120" activeTab="1" xr2:uid="{B7CF2435-4AB2-8449-A283-99C1C1B4CF66}"/>
   </bookViews>
   <sheets>
     <sheet name="lookup_table" sheetId="8" r:id="rId1"/>
@@ -30,8 +30,8 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">[1]Tabelle2!$B$3:$B$27</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">[1]Tabelle2!$C$3:$C$27</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Tabelle2!$E$3:$E$33</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Tabelle2!$F$3:$F$33</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">[2]Tabelle2!$D$3:$D$191</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">[2]Tabelle2!$E$3:$E$191</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">[1]Tabelle2!$B$12:$B$19</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">[1]Tabelle2!$B$20:$B$27</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">[1]Tabelle2!$B$3:$B$11</definedName>
@@ -48,23 +48,31 @@
     <definedName name="_xlchart.v1.24" hidden="1">[2]Tabelle2!$K$3:$K$191</definedName>
     <definedName name="_xlchart.v1.25" hidden="1">[2]Tabelle2!$L$3:$L$191</definedName>
     <definedName name="_xlchart.v1.26" hidden="1">[2]Tabelle2!$M$3:$M$191</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Tabelle1!$D$2</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Tabelle1!$D$3:$D$15</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Tabelle1!$E$2</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">[1]Tabelle2!$J$3:$J$27</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">[1]Tabelle2!$K$3:$K$27</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">[1]Tabelle2!$L$3:$L$27</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">[1]Tabelle2!$E$3:$E$27</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Tabelle1!$E$3:$E$15</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Tabelle1!$F$2</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Tabelle1!$F$3:$F$15</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Tabelle1!$G$3:$G$36</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Tabelle1!$H$3:$H$36</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Tabelle1!$I$3:$I$36</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Tabelle1!$J$3:$J$36</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">[2]Tabelle2!$B$3:$B$191</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">[2]Tabelle2!$C$3:$C$191</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">[2]Tabelle2!$D$3:$D$191</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">[2]Tabelle2!$E$3:$E$191</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Tabelle2!$C$3:$C$33</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Tabelle2!$D$3:$D$33</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">[1]Tabelle2!$M$3:$M$27</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">[2]Tabelle2!$J$3:$J$191</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">[2]Tabelle2!$K$3:$K$191</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">[2]Tabelle2!$L$3:$L$191</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">[2]Tabelle2!$M$3:$M$191</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Tabelle1!$G$3:$G$36</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Tabelle1!$H$3:$H$36</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Tabelle1!$I$3:$I$36</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Tabelle1!$J$3:$J$36</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Tabelle1!$D$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Tabelle2!$C$3:$C$33</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Tabelle1!$D$3:$D$15</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Tabelle1!$E$2</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Tabelle1!$E$3:$E$15</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Tabelle1!$F$2</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Tabelle1!$F$3:$F$15</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Tabelle2!$D$3:$D$33</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Tabelle2!$E$3:$E$33</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Tabelle2!$F$3:$F$33</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">[2]Tabelle2!$B$3:$B$191</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">[2]Tabelle2!$C$3:$C$191</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2287,7 +2295,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -3100,7 +3108,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
@@ -3110,13 +3118,13 @@
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3"/>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
@@ -3126,13 +3134,13 @@
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7"/>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
@@ -3142,13 +3150,13 @@
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11"/>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
@@ -3158,7 +3166,7 @@
     </cx:data>
     <cx:data id="14">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4187,17 +4195,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.28</cx:f>
+        <cx:f>_xlchart.v1.40</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.30</cx:f>
+        <cx:f>_xlchart.v1.42</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.32</cx:f>
+        <cx:f>_xlchart.v1.44</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4268,7 +4276,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24BF4607-F4E8-E345-97F3-975C8A945A06}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.27</cx:f>
+              <cx:f>_xlchart.v1.39</cx:f>
               <cx:v>rcp26</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4281,7 +4289,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B15400F1-0218-BE43-9F95-AD4EAABB47CD}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.29</cx:f>
+              <cx:f>_xlchart.v1.41</cx:f>
               <cx:v>rcp45</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4294,7 +4302,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{99A6A248-8D06-4B4A-861B-9E311114F9A0}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.31</cx:f>
+              <cx:f>_xlchart.v1.43</cx:f>
               <cx:v>rcp85</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4360,22 +4368,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.33</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.34</cx:f>
+        <cx:f>_xlchart.v1.36</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.35</cx:f>
+        <cx:f>_xlchart.v1.37</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.36</cx:f>
+        <cx:f>_xlchart.v1.38</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8658,7 +8666,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE2E835-29F0-6D41-9B7E-CBE95F59253D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{046980F5-1704-F8BB-6927-DBD6B2746A1D}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -8703,7 +8711,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9303008" cy="6019593"/>
+    <xdr:ext cx="9304421" cy="6015789"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
@@ -8769,7 +8777,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE29E545-24A1-0311-6E2E-16080F03EEA7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25624F71-0E2B-E1CB-44FC-0C6A7492A11E}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -8780,7 +8788,7 @@
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="0"/>
-          <a:ext cx="9303008" cy="6019593"/>
+          <a:ext cx="9304421" cy="6015789"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -8880,7 +8888,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76C0F252-2BF4-D15E-AD2B-FFE86852B0D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B8A96AD-7BB9-36D1-5BC9-7A4194A42716}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -9603,12 +9611,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3"/>
-          <cell r="K3"/>
-          <cell r="L3"/>
-          <cell r="M3"/>
-        </row>
         <row r="4">
           <cell r="B4">
             <v>2068</v>
@@ -9616,9 +9618,6 @@
           <cell r="J4">
             <v>0.953297643723377</v>
           </cell>
-          <cell r="K4"/>
-          <cell r="L4"/>
-          <cell r="M4"/>
         </row>
         <row r="5">
           <cell r="B5">
@@ -9633,8 +9632,6 @@
           <cell r="K5">
             <v>1.12528774120191</v>
           </cell>
-          <cell r="L5"/>
-          <cell r="M5"/>
         </row>
         <row r="6">
           <cell r="B6">
@@ -9643,9 +9640,6 @@
           <cell r="J6">
             <v>0.962655414052216</v>
           </cell>
-          <cell r="K6"/>
-          <cell r="L6"/>
-          <cell r="M6"/>
         </row>
         <row r="7">
           <cell r="B7">
@@ -9660,20 +9654,6 @@
           <cell r="K7">
             <v>0.75275346345142902</v>
           </cell>
-          <cell r="L7"/>
-          <cell r="M7"/>
-        </row>
-        <row r="8">
-          <cell r="J8"/>
-          <cell r="K8"/>
-          <cell r="L8"/>
-          <cell r="M8"/>
-        </row>
-        <row r="9">
-          <cell r="J9"/>
-          <cell r="K9"/>
-          <cell r="L9"/>
-          <cell r="M9"/>
         </row>
         <row r="10">
           <cell r="B10">
@@ -9688,26 +9668,6 @@
           <cell r="K10">
             <v>1.2996490999999999</v>
           </cell>
-          <cell r="L10"/>
-          <cell r="M10"/>
-        </row>
-        <row r="11">
-          <cell r="J11"/>
-          <cell r="K11"/>
-          <cell r="L11"/>
-          <cell r="M11"/>
-        </row>
-        <row r="12">
-          <cell r="J12"/>
-          <cell r="K12"/>
-          <cell r="L12"/>
-          <cell r="M12"/>
-        </row>
-        <row r="13">
-          <cell r="J13"/>
-          <cell r="K13"/>
-          <cell r="L13"/>
-          <cell r="M13"/>
         </row>
         <row r="14">
           <cell r="B14">
@@ -9716,9 +9676,6 @@
           <cell r="J14">
             <v>1.1676970687033701</v>
           </cell>
-          <cell r="K14"/>
-          <cell r="L14"/>
-          <cell r="M14"/>
         </row>
         <row r="15">
           <cell r="B15">
@@ -9733,8 +9690,6 @@
           <cell r="K15">
             <v>2.1459751510413598</v>
           </cell>
-          <cell r="L15"/>
-          <cell r="M15"/>
         </row>
         <row r="16">
           <cell r="B16">
@@ -9749,8 +9704,6 @@
           <cell r="K16">
             <v>1.8127139886377099</v>
           </cell>
-          <cell r="L16"/>
-          <cell r="M16"/>
         </row>
         <row r="17">
           <cell r="B17">
@@ -9765,8 +9718,6 @@
           <cell r="K17">
             <v>1.8433555303092599</v>
           </cell>
-          <cell r="L17"/>
-          <cell r="M17"/>
         </row>
         <row r="18">
           <cell r="B18">
@@ -9781,8 +9732,6 @@
           <cell r="K18">
             <v>1.2746751758441699</v>
           </cell>
-          <cell r="L18"/>
-          <cell r="M18"/>
         </row>
         <row r="19">
           <cell r="B19">
@@ -9791,15 +9740,6 @@
           <cell r="J19">
             <v>0.50765736677745898</v>
           </cell>
-          <cell r="K19"/>
-          <cell r="L19"/>
-          <cell r="M19"/>
-        </row>
-        <row r="20">
-          <cell r="J20"/>
-          <cell r="K20"/>
-          <cell r="L20"/>
-          <cell r="M20"/>
         </row>
         <row r="21">
           <cell r="B21">
@@ -9814,8 +9754,6 @@
           <cell r="K21">
             <v>3.1213066025999701</v>
           </cell>
-          <cell r="L21"/>
-          <cell r="M21"/>
         </row>
         <row r="22">
           <cell r="B22">
@@ -9830,8 +9768,6 @@
           <cell r="K22">
             <v>1.3981454217936999</v>
           </cell>
-          <cell r="L22"/>
-          <cell r="M22"/>
         </row>
         <row r="23">
           <cell r="B23">
@@ -9846,8 +9782,6 @@
           <cell r="K23">
             <v>1.67016129100406</v>
           </cell>
-          <cell r="L23"/>
-          <cell r="M23"/>
         </row>
         <row r="24">
           <cell r="B24">
@@ -9862,8 +9796,6 @@
           <cell r="K24">
             <v>1.0728179942746401</v>
           </cell>
-          <cell r="L24"/>
-          <cell r="M24"/>
         </row>
         <row r="25">
           <cell r="B25">
@@ -9878,8 +9810,6 @@
           <cell r="K25">
             <v>1.6734034587411499</v>
           </cell>
-          <cell r="L25"/>
-          <cell r="M25"/>
         </row>
         <row r="26">
           <cell r="B26">
@@ -9894,8 +9824,6 @@
           <cell r="K26">
             <v>0.94311847540844496</v>
           </cell>
-          <cell r="L26"/>
-          <cell r="M26"/>
         </row>
         <row r="27">
           <cell r="B27">
@@ -9910,8 +9838,6 @@
           <cell r="K27">
             <v>1.4934826904101901</v>
           </cell>
-          <cell r="L27"/>
-          <cell r="M27"/>
         </row>
         <row r="28">
           <cell r="B28">
@@ -9920,9 +9846,6 @@
           <cell r="J28">
             <v>1.0283560461610499</v>
           </cell>
-          <cell r="K28"/>
-          <cell r="L28"/>
-          <cell r="M28"/>
         </row>
         <row r="29">
           <cell r="B29">
@@ -9937,8 +9860,6 @@
           <cell r="K29">
             <v>0.45363177546752198</v>
           </cell>
-          <cell r="L29"/>
-          <cell r="M29"/>
         </row>
         <row r="30">
           <cell r="B30">
@@ -9953,8 +9874,6 @@
           <cell r="K30">
             <v>0.91811225325973</v>
           </cell>
-          <cell r="L30"/>
-          <cell r="M30"/>
         </row>
         <row r="31">
           <cell r="B31">
@@ -9963,9 +9882,6 @@
           <cell r="J31">
             <v>1.0129333473675</v>
           </cell>
-          <cell r="K31"/>
-          <cell r="L31"/>
-          <cell r="M31"/>
         </row>
         <row r="32">
           <cell r="B32">
@@ -9980,8 +9896,6 @@
           <cell r="K32">
             <v>0.93398420658576498</v>
           </cell>
-          <cell r="L32"/>
-          <cell r="M32"/>
         </row>
         <row r="33">
           <cell r="B33">
@@ -9996,8 +9910,6 @@
           <cell r="K33">
             <v>1.9070619275280301</v>
           </cell>
-          <cell r="L33"/>
-          <cell r="M33"/>
         </row>
         <row r="34">
           <cell r="B34">
@@ -10012,14 +9924,6 @@
           <cell r="K34">
             <v>1.03584774279575</v>
           </cell>
-          <cell r="L34"/>
-          <cell r="M34"/>
-        </row>
-        <row r="35">
-          <cell r="J35"/>
-          <cell r="K35"/>
-          <cell r="L35"/>
-          <cell r="M35"/>
         </row>
         <row r="36">
           <cell r="B36">
@@ -10034,14 +9938,6 @@
           <cell r="K36">
             <v>1.1211079653474301</v>
           </cell>
-          <cell r="L36"/>
-          <cell r="M36"/>
-        </row>
-        <row r="37">
-          <cell r="J37"/>
-          <cell r="K37"/>
-          <cell r="L37"/>
-          <cell r="M37"/>
         </row>
         <row r="38">
           <cell r="B38">
@@ -10050,9 +9946,6 @@
           <cell r="J38">
             <v>1.47924744842162</v>
           </cell>
-          <cell r="K38"/>
-          <cell r="L38"/>
-          <cell r="M38"/>
         </row>
         <row r="39">
           <cell r="B39">
@@ -10067,8 +9960,6 @@
           <cell r="K39">
             <v>1.47625627991256</v>
           </cell>
-          <cell r="L39"/>
-          <cell r="M39"/>
         </row>
         <row r="40">
           <cell r="B40">
@@ -10083,8 +9974,6 @@
           <cell r="K40">
             <v>1.22094780806839</v>
           </cell>
-          <cell r="L40"/>
-          <cell r="M40"/>
         </row>
         <row r="41">
           <cell r="B41">
@@ -10099,8 +9988,6 @@
           <cell r="K41">
             <v>1.7052057166927399</v>
           </cell>
-          <cell r="L41"/>
-          <cell r="M41"/>
         </row>
         <row r="42">
           <cell r="B42">
@@ -10109,9 +9996,6 @@
           <cell r="J42">
             <v>0.81285915249012197</v>
           </cell>
-          <cell r="K42"/>
-          <cell r="L42"/>
-          <cell r="M42"/>
         </row>
         <row r="43">
           <cell r="B43">
@@ -10120,9 +10004,6 @@
           <cell r="J43">
             <v>0.85479150373844803</v>
           </cell>
-          <cell r="K43"/>
-          <cell r="L43"/>
-          <cell r="M43"/>
         </row>
         <row r="44">
           <cell r="B44">
@@ -10131,9 +10012,6 @@
           <cell r="J44">
             <v>1.24668562684192</v>
           </cell>
-          <cell r="K44"/>
-          <cell r="L44"/>
-          <cell r="M44"/>
         </row>
         <row r="45">
           <cell r="B45">
@@ -10174,8 +10052,6 @@
           <cell r="K46">
             <v>0.99413149999999995</v>
           </cell>
-          <cell r="L46"/>
-          <cell r="M46"/>
         </row>
         <row r="47">
           <cell r="B47">
@@ -10190,8 +10066,6 @@
           <cell r="K47">
             <v>1.2139563001517599</v>
           </cell>
-          <cell r="L47"/>
-          <cell r="M47"/>
         </row>
         <row r="48">
           <cell r="B48">
@@ -10200,9 +10074,6 @@
           <cell r="J48">
             <v>0.31548891067506302</v>
           </cell>
-          <cell r="K48"/>
-          <cell r="L48"/>
-          <cell r="M48"/>
         </row>
         <row r="49">
           <cell r="B49">
@@ -10217,8 +10088,6 @@
           <cell r="K49">
             <v>1.43005460103351</v>
           </cell>
-          <cell r="L49"/>
-          <cell r="M49"/>
         </row>
         <row r="50">
           <cell r="B50">
@@ -10227,9 +10096,6 @@
           <cell r="J50">
             <v>1.58398556179473</v>
           </cell>
-          <cell r="K50"/>
-          <cell r="L50"/>
-          <cell r="M50"/>
         </row>
         <row r="51">
           <cell r="B51">
@@ -10238,9 +10104,6 @@
           <cell r="J51">
             <v>1.5601286800869001</v>
           </cell>
-          <cell r="K51"/>
-          <cell r="L51"/>
-          <cell r="M51"/>
         </row>
         <row r="52">
           <cell r="B52">
@@ -10249,9 +10112,6 @@
           <cell r="J52">
             <v>0.89465247498328804</v>
           </cell>
-          <cell r="K52"/>
-          <cell r="L52"/>
-          <cell r="M52"/>
         </row>
         <row r="53">
           <cell r="B53">
@@ -10260,9 +10120,6 @@
           <cell r="J53">
             <v>1.4470739576551801</v>
           </cell>
-          <cell r="K53"/>
-          <cell r="L53"/>
-          <cell r="M53"/>
         </row>
         <row r="54">
           <cell r="B54">
@@ -10271,9 +10128,6 @@
           <cell r="J54">
             <v>0.93532776547523599</v>
           </cell>
-          <cell r="K54"/>
-          <cell r="L54"/>
-          <cell r="M54"/>
         </row>
         <row r="55">
           <cell r="B55">
@@ -10288,20 +10142,6 @@
           <cell r="K55">
             <v>1.4829433865017501</v>
           </cell>
-          <cell r="L55"/>
-          <cell r="M55"/>
-        </row>
-        <row r="56">
-          <cell r="J56"/>
-          <cell r="K56"/>
-          <cell r="L56"/>
-          <cell r="M56"/>
-        </row>
-        <row r="57">
-          <cell r="J57"/>
-          <cell r="K57"/>
-          <cell r="L57"/>
-          <cell r="M57"/>
         </row>
         <row r="58">
           <cell r="B58">
@@ -10316,8 +10156,6 @@
           <cell r="K58">
             <v>1.7895930232263599</v>
           </cell>
-          <cell r="L58"/>
-          <cell r="M58"/>
         </row>
         <row r="59">
           <cell r="B59">
@@ -10332,8 +10170,6 @@
           <cell r="K59">
             <v>1.8116578232415801</v>
           </cell>
-          <cell r="L59"/>
-          <cell r="M59"/>
         </row>
         <row r="60">
           <cell r="B60">
@@ -10354,7 +10190,6 @@
           <cell r="L60">
             <v>3.0059425348697002</v>
           </cell>
-          <cell r="M60"/>
         </row>
         <row r="61">
           <cell r="B61">
@@ -10369,8 +10204,6 @@
           <cell r="K61">
             <v>1.7521867119608101</v>
           </cell>
-          <cell r="L61"/>
-          <cell r="M61"/>
         </row>
         <row r="62">
           <cell r="B62">
@@ -10385,8 +10218,6 @@
           <cell r="K62">
             <v>1.1976161575342901</v>
           </cell>
-          <cell r="L62"/>
-          <cell r="M62"/>
         </row>
         <row r="63">
           <cell r="B63">
@@ -10401,8 +10232,6 @@
           <cell r="K63">
             <v>1.79025508687392</v>
           </cell>
-          <cell r="L63"/>
-          <cell r="M63"/>
         </row>
         <row r="64">
           <cell r="B64">
@@ -10417,8 +10246,6 @@
           <cell r="K64">
             <v>1.8836058328781899</v>
           </cell>
-          <cell r="L64"/>
-          <cell r="M64"/>
         </row>
         <row r="65">
           <cell r="B65">
@@ -10439,7 +10266,6 @@
           <cell r="L65">
             <v>4.2916051539023199</v>
           </cell>
-          <cell r="M65"/>
         </row>
         <row r="66">
           <cell r="B66">
@@ -10460,7 +10286,6 @@
           <cell r="L66">
             <v>2.0659365442925499</v>
           </cell>
-          <cell r="M66"/>
         </row>
         <row r="67">
           <cell r="B67">
@@ -10481,7 +10306,6 @@
           <cell r="L67">
             <v>2.07600407171268</v>
           </cell>
-          <cell r="M67"/>
         </row>
         <row r="68">
           <cell r="B68">
@@ -10502,7 +10326,6 @@
           <cell r="L68">
             <v>2.46145115976516</v>
           </cell>
-          <cell r="M68"/>
         </row>
         <row r="69">
           <cell r="B69">
@@ -10523,7 +10346,6 @@
           <cell r="L69">
             <v>2.95128872598479</v>
           </cell>
-          <cell r="M69"/>
         </row>
         <row r="70">
           <cell r="B70">
@@ -10544,7 +10366,6 @@
           <cell r="L70">
             <v>2.4659900553596299</v>
           </cell>
-          <cell r="M70"/>
         </row>
         <row r="71">
           <cell r="B71">
@@ -10565,7 +10386,6 @@
           <cell r="L71">
             <v>1.9276448337221399</v>
           </cell>
-          <cell r="M71"/>
         </row>
         <row r="72">
           <cell r="B72">
@@ -10586,7 +10406,6 @@
           <cell r="L72">
             <v>2.2183875868211</v>
           </cell>
-          <cell r="M72"/>
         </row>
         <row r="73">
           <cell r="B73">
@@ -10659,7 +10478,6 @@
           <cell r="L75">
             <v>1.7990900046379901</v>
           </cell>
-          <cell r="M75"/>
         </row>
         <row r="76">
           <cell r="B76">
@@ -10680,7 +10498,6 @@
           <cell r="L76">
             <v>2.3771028757036698</v>
           </cell>
-          <cell r="M76"/>
         </row>
         <row r="77">
           <cell r="B77">
@@ -10701,7 +10518,6 @@
           <cell r="L77">
             <v>1.64459827038435</v>
           </cell>
-          <cell r="M77"/>
         </row>
         <row r="78">
           <cell r="B78">
@@ -10722,7 +10538,6 @@
           <cell r="L78">
             <v>2.4737583558019298</v>
           </cell>
-          <cell r="M78"/>
         </row>
         <row r="79">
           <cell r="B79">
@@ -10737,8 +10552,6 @@
           <cell r="K79">
             <v>1.1256945521228801</v>
           </cell>
-          <cell r="L79"/>
-          <cell r="M79"/>
         </row>
         <row r="80">
           <cell r="B80">
@@ -10753,8 +10566,6 @@
           <cell r="K80">
             <v>1.42677008310954</v>
           </cell>
-          <cell r="L80"/>
-          <cell r="M80"/>
         </row>
         <row r="81">
           <cell r="B81">
@@ -10775,7 +10586,6 @@
           <cell r="L81">
             <v>2.1591106380818599</v>
           </cell>
-          <cell r="M81"/>
         </row>
         <row r="82">
           <cell r="B82">
@@ -10790,8 +10600,6 @@
           <cell r="K82">
             <v>1.6772889300680101</v>
           </cell>
-          <cell r="L82"/>
-          <cell r="M82"/>
         </row>
         <row r="83">
           <cell r="B83">
@@ -10806,8 +10614,6 @@
           <cell r="K83">
             <v>1.65557634817044</v>
           </cell>
-          <cell r="L83"/>
-          <cell r="M83"/>
         </row>
         <row r="84">
           <cell r="B84">
@@ -10822,8 +10628,6 @@
           <cell r="K84">
             <v>1.79784619645486</v>
           </cell>
-          <cell r="L84"/>
-          <cell r="M84"/>
         </row>
         <row r="85">
           <cell r="B85">
@@ -10838,8 +10642,6 @@
           <cell r="K85">
             <v>1.7099448768059999</v>
           </cell>
-          <cell r="L85"/>
-          <cell r="M85"/>
         </row>
         <row r="86">
           <cell r="B86">
@@ -10860,7 +10662,6 @@
           <cell r="L86">
             <v>2.7137934503127701</v>
           </cell>
-          <cell r="M86"/>
         </row>
         <row r="87">
           <cell r="B87">
@@ -10881,7 +10682,6 @@
           <cell r="L87">
             <v>2.6473017385885602</v>
           </cell>
-          <cell r="M87"/>
         </row>
         <row r="88">
           <cell r="B88">
@@ -10896,8 +10696,6 @@
           <cell r="K88">
             <v>1.4064785184664499</v>
           </cell>
-          <cell r="L88"/>
-          <cell r="M88"/>
         </row>
         <row r="89">
           <cell r="B89">
@@ -10912,8 +10710,6 @@
           <cell r="K89">
             <v>1.8829193396530901</v>
           </cell>
-          <cell r="L89"/>
-          <cell r="M89"/>
         </row>
         <row r="90">
           <cell r="B90">
@@ -10928,8 +10724,6 @@
           <cell r="K90">
             <v>1.9885308508852599</v>
           </cell>
-          <cell r="L90"/>
-          <cell r="M90"/>
         </row>
         <row r="91">
           <cell r="B91">
@@ -10950,7 +10744,6 @@
           <cell r="L91">
             <v>2.7629134999999998</v>
           </cell>
-          <cell r="M91"/>
         </row>
         <row r="92">
           <cell r="B92">
@@ -10971,7 +10764,6 @@
           <cell r="L92">
             <v>2.61799366766664</v>
           </cell>
-          <cell r="M92"/>
         </row>
         <row r="93">
           <cell r="B93">
@@ -10986,8 +10778,6 @@
           <cell r="K93">
             <v>0.74702986611260902</v>
           </cell>
-          <cell r="L93"/>
-          <cell r="M93"/>
         </row>
         <row r="94">
           <cell r="B94">
@@ -11002,8 +10792,6 @@
           <cell r="K94">
             <v>1.81199906667073</v>
           </cell>
-          <cell r="L94"/>
-          <cell r="M94"/>
         </row>
         <row r="95">
           <cell r="B95">
@@ -11018,8 +10806,6 @@
           <cell r="K95">
             <v>2.3510983361137998</v>
           </cell>
-          <cell r="L95"/>
-          <cell r="M95"/>
         </row>
         <row r="96">
           <cell r="B96">
@@ -11034,8 +10820,6 @@
           <cell r="K96">
             <v>1.8110792384853101</v>
           </cell>
-          <cell r="L96"/>
-          <cell r="M96"/>
         </row>
         <row r="97">
           <cell r="B97">
@@ -11050,8 +10834,6 @@
           <cell r="K97">
             <v>1.5849269976389799</v>
           </cell>
-          <cell r="L97"/>
-          <cell r="M97"/>
         </row>
         <row r="98">
           <cell r="B98">
@@ -11066,8 +10848,6 @@
           <cell r="K98">
             <v>1.61900668674048</v>
           </cell>
-          <cell r="L98"/>
-          <cell r="M98"/>
         </row>
         <row r="99">
           <cell r="B99">
@@ -11082,8 +10862,6 @@
           <cell r="K99">
             <v>1.3695843568142401</v>
           </cell>
-          <cell r="L99"/>
-          <cell r="M99"/>
         </row>
         <row r="100">
           <cell r="B100">
@@ -11098,8 +10876,6 @@
           <cell r="K100">
             <v>1.71808351940573</v>
           </cell>
-          <cell r="L100"/>
-          <cell r="M100"/>
         </row>
         <row r="101">
           <cell r="B101">
@@ -11114,8 +10890,6 @@
           <cell r="K101">
             <v>2.1603128362584698</v>
           </cell>
-          <cell r="L101"/>
-          <cell r="M101"/>
         </row>
         <row r="102">
           <cell r="B102">
@@ -11130,8 +10904,6 @@
           <cell r="K102">
             <v>1.9302608195684401</v>
           </cell>
-          <cell r="L102"/>
-          <cell r="M102"/>
         </row>
         <row r="103">
           <cell r="B103">
@@ -11152,7 +10924,6 @@
           <cell r="L103">
             <v>3.1708323798723201</v>
           </cell>
-          <cell r="M103"/>
         </row>
         <row r="104">
           <cell r="B104">
@@ -11225,7 +10996,6 @@
           <cell r="L106">
             <v>3.02139535831243</v>
           </cell>
-          <cell r="M106"/>
         </row>
         <row r="107">
           <cell r="B107">
@@ -11246,7 +11016,6 @@
           <cell r="L107">
             <v>2.7878231845461698</v>
           </cell>
-          <cell r="M107"/>
         </row>
         <row r="108">
           <cell r="B108">
@@ -11267,7 +11036,6 @@
           <cell r="L108">
             <v>3.1576496725510599</v>
           </cell>
-          <cell r="M108"/>
         </row>
         <row r="109">
           <cell r="B109">
@@ -11276,9 +11044,6 @@
           <cell r="J109">
             <v>1.5657428882740401</v>
           </cell>
-          <cell r="K109"/>
-          <cell r="L109"/>
-          <cell r="M109"/>
         </row>
         <row r="110">
           <cell r="B110">
@@ -11293,8 +11058,6 @@
           <cell r="K110">
             <v>1.8104741339919299</v>
           </cell>
-          <cell r="L110"/>
-          <cell r="M110"/>
         </row>
         <row r="111">
           <cell r="B111">
@@ -11315,7 +11078,6 @@
           <cell r="L111">
             <v>4.1255501015432303</v>
           </cell>
-          <cell r="M111"/>
         </row>
         <row r="112">
           <cell r="B112">
@@ -11674,7 +11436,6 @@
           <cell r="L125">
             <v>2.1705614599349499</v>
           </cell>
-          <cell r="M125"/>
         </row>
         <row r="126">
           <cell r="B126">
@@ -11695,7 +11456,6 @@
           <cell r="L126">
             <v>2.21875868903268</v>
           </cell>
-          <cell r="M126"/>
         </row>
         <row r="127">
           <cell r="B127">
@@ -11716,7 +11476,6 @@
           <cell r="L127">
             <v>3.0087400281739001</v>
           </cell>
-          <cell r="M127"/>
         </row>
         <row r="128">
           <cell r="B128">
@@ -11737,7 +11496,6 @@
           <cell r="L128">
             <v>2.5273760401932899</v>
           </cell>
-          <cell r="M128"/>
         </row>
         <row r="129">
           <cell r="B129">
@@ -11758,7 +11516,6 @@
           <cell r="L129">
             <v>2.6335885440636302</v>
           </cell>
-          <cell r="M129"/>
         </row>
         <row r="130">
           <cell r="B130">
@@ -11779,7 +11536,6 @@
           <cell r="L130">
             <v>2.3055320339923799</v>
           </cell>
-          <cell r="M130"/>
         </row>
         <row r="131">
           <cell r="B131">
@@ -11800,7 +11556,6 @@
           <cell r="L131">
             <v>2.8297057592542201</v>
           </cell>
-          <cell r="M131"/>
         </row>
         <row r="132">
           <cell r="B132">
@@ -11821,7 +11576,6 @@
           <cell r="L132">
             <v>3.20905435545248</v>
           </cell>
-          <cell r="M132"/>
         </row>
         <row r="133">
           <cell r="B133">
@@ -11920,7 +11674,6 @@
           <cell r="L136">
             <v>2.4212512758043401</v>
           </cell>
-          <cell r="M136"/>
         </row>
         <row r="137">
           <cell r="B137">
@@ -11941,7 +11694,6 @@
           <cell r="L137">
             <v>3.4698040573684898</v>
           </cell>
-          <cell r="M137"/>
         </row>
         <row r="138">
           <cell r="B138">
@@ -11956,8 +11708,6 @@
           <cell r="K138">
             <v>2.2215974851091702</v>
           </cell>
-          <cell r="L138"/>
-          <cell r="M138"/>
         </row>
         <row r="139">
           <cell r="B139">
@@ -11966,9 +11716,6 @@
           <cell r="J139">
             <v>1.4871546851264099</v>
           </cell>
-          <cell r="K139"/>
-          <cell r="L139"/>
-          <cell r="M139"/>
         </row>
         <row r="140">
           <cell r="B140">
@@ -11989,7 +11736,6 @@
           <cell r="L140">
             <v>2.76461721959198</v>
           </cell>
-          <cell r="M140"/>
         </row>
         <row r="141">
           <cell r="B141">
@@ -12010,7 +11756,6 @@
           <cell r="L141">
             <v>3.0094896104601001</v>
           </cell>
-          <cell r="M141"/>
         </row>
         <row r="142">
           <cell r="B142">
@@ -12031,7 +11776,6 @@
           <cell r="L142">
             <v>2.2740586286362601</v>
           </cell>
-          <cell r="M142"/>
         </row>
         <row r="143">
           <cell r="B143">
@@ -12046,8 +11790,6 @@
           <cell r="K143">
             <v>2.1390993330213699</v>
           </cell>
-          <cell r="L143"/>
-          <cell r="M143"/>
         </row>
         <row r="144">
           <cell r="B144">
@@ -12068,7 +11810,6 @@
           <cell r="L144">
             <v>3.6687247613706999</v>
           </cell>
-          <cell r="M144"/>
         </row>
         <row r="145">
           <cell r="B145">
@@ -12219,7 +11960,6 @@
           <cell r="L150">
             <v>3.30951525175441</v>
           </cell>
-          <cell r="M150"/>
         </row>
         <row r="151">
           <cell r="B151">
@@ -12240,7 +11980,6 @@
           <cell r="L151">
             <v>2.9504145044591001</v>
           </cell>
-          <cell r="M151"/>
         </row>
         <row r="152">
           <cell r="B152">
@@ -12651,7 +12390,6 @@
           <cell r="L167">
             <v>2.2516428417629699</v>
           </cell>
-          <cell r="M167"/>
         </row>
         <row r="168">
           <cell r="B168">
@@ -12750,7 +12488,6 @@
           <cell r="L171">
             <v>3.04848111038363</v>
           </cell>
-          <cell r="M171"/>
         </row>
         <row r="172">
           <cell r="B172">
@@ -12849,7 +12586,6 @@
           <cell r="L175">
             <v>2.5286943670620601</v>
           </cell>
-          <cell r="M175"/>
         </row>
         <row r="176">
           <cell r="B176">
@@ -12870,7 +12606,6 @@
           <cell r="L176">
             <v>2.7677175902520599</v>
           </cell>
-          <cell r="M176"/>
         </row>
         <row r="177">
           <cell r="B177">
@@ -12891,7 +12626,6 @@
           <cell r="L177">
             <v>2.9216101985538199</v>
           </cell>
-          <cell r="M177"/>
         </row>
         <row r="178">
           <cell r="B178">
@@ -12964,7 +12698,6 @@
           <cell r="L180">
             <v>2.3987316555447</v>
           </cell>
-          <cell r="M180"/>
         </row>
         <row r="181">
           <cell r="B181">
@@ -13011,7 +12744,6 @@
           <cell r="L182">
             <v>3.49936630814164</v>
           </cell>
-          <cell r="M182"/>
         </row>
         <row r="183">
           <cell r="B183">
@@ -13032,7 +12764,6 @@
           <cell r="L183">
             <v>3.3262258100273101</v>
           </cell>
-          <cell r="M183"/>
         </row>
         <row r="184">
           <cell r="B184">
@@ -13053,7 +12784,6 @@
           <cell r="L184">
             <v>2.8145093766053302</v>
           </cell>
-          <cell r="M184"/>
         </row>
         <row r="185">
           <cell r="B185">
@@ -13074,7 +12804,6 @@
           <cell r="L185">
             <v>2.8472741021049801</v>
           </cell>
-          <cell r="M185"/>
         </row>
         <row r="186">
           <cell r="B186">
@@ -13147,7 +12876,6 @@
           <cell r="L188">
             <v>3.3017069074842902</v>
           </cell>
-          <cell r="M188"/>
         </row>
         <row r="189">
           <cell r="B189">
@@ -13168,7 +12896,6 @@
           <cell r="L189">
             <v>3.3375443506061302</v>
           </cell>
-          <cell r="M189"/>
         </row>
         <row r="190">
           <cell r="B190">
@@ -13527,8 +13254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE29186-7B7C-D348-AEA4-5951DF45B0E5}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13999,10 +13726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8388F6E0-5660-DB40-B6C7-A98F3137AF83}">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14545,7 +14272,7 @@
       </c>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -14591,7 +14318,7 @@
       </c>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -14637,7 +14364,7 @@
       </c>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -14683,7 +14410,7 @@
       </c>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -14719,7 +14446,7 @@
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -14755,7 +14482,7 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -14810,8 +14537,9 @@
       <c r="R22" s="3">
         <v>3.0102582</v>
       </c>
+      <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -14866,8 +14594,9 @@
       <c r="R23" s="3">
         <v>3.5986015999999998</v>
       </c>
+      <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -14923,7 +14652,7 @@
         <v>3.9668462</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -14969,7 +14698,7 @@
       </c>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -15015,7 +14744,7 @@
       </c>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -15071,7 +14800,7 @@
         <v>3.250985</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -15127,7 +14856,7 @@
         <v>3.6632657000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -15183,7 +14912,7 @@
         <v>3.5443655999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -15239,7 +14968,7 @@
         <v>2.1218149999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -15295,7 +15024,7 @@
         <v>3.1780202000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Added lookup table for CMIP6 OEKS15 GWLs
</commit_message>
<xml_diff>
--- a/data/gwl_lists/GWLs_CMIP5_OEKS15.xlsx
+++ b/data/gwl_lists/GWLs_CMIP5_OEKS15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbecsi/Desktop/Arbeit/Qgis/data/AAR2/GWLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859FE6EE-AAAA-F646-8C4A-D5557ADCEF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A90744A-6723-1446-81D3-A072BC41B0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22120" activeTab="1" xr2:uid="{B7CF2435-4AB2-8449-A283-99C1C1B4CF66}"/>
   </bookViews>
@@ -30,8 +30,8 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">[1]Tabelle2!$B$3:$B$27</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">[1]Tabelle2!$C$3:$C$27</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">[2]Tabelle2!$D$3:$D$191</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">[2]Tabelle2!$E$3:$E$191</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Tabelle2!$E$3:$E$33</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Tabelle2!$F$3:$F$33</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">[1]Tabelle2!$B$12:$B$19</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">[1]Tabelle2!$B$20:$B$27</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">[1]Tabelle2!$B$3:$B$11</definedName>
@@ -57,22 +57,22 @@
     <definedName name="_xlchart.v1.32" hidden="1">[2]Tabelle2!$K$3:$K$191</definedName>
     <definedName name="_xlchart.v1.33" hidden="1">[2]Tabelle2!$L$3:$L$191</definedName>
     <definedName name="_xlchart.v1.34" hidden="1">[2]Tabelle2!$M$3:$M$191</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Tabelle1!$G$3:$G$36</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Tabelle1!$H$3:$H$36</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Tabelle1!$I$3:$I$36</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Tabelle1!$J$3:$J$36</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Tabelle1!$D$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Tabelle2!$C$3:$C$33</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Tabelle1!$D$3:$D$15</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Tabelle1!$E$2</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Tabelle1!$E$3:$E$15</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Tabelle1!$F$2</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Tabelle1!$F$3:$F$15</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Tabelle2!$D$3:$D$33</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Tabelle2!$E$3:$E$33</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Tabelle2!$F$3:$F$33</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">[2]Tabelle2!$B$3:$B$191</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">[2]Tabelle2!$C$3:$C$191</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Tabelle1!$D$2</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Tabelle1!$D$3:$D$15</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Tabelle1!$E$2</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Tabelle1!$E$3:$E$15</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Tabelle1!$F$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">[2]Tabelle2!$B$3:$B$191</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Tabelle1!$F$3:$F$15</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Tabelle1!$G$3:$G$36</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Tabelle1!$H$3:$H$36</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Tabelle1!$I$3:$I$36</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Tabelle1!$J$3:$J$36</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">[2]Tabelle2!$C$3:$C$191</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">[2]Tabelle2!$D$3:$D$191</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">[2]Tabelle2!$E$3:$E$191</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Tabelle2!$C$3:$C$33</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Tabelle2!$D$3:$D$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3108,7 +3108,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
@@ -3118,13 +3118,13 @@
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3"/>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
@@ -3134,13 +3134,13 @@
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7"/>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
@@ -3150,13 +3150,13 @@
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11"/>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
@@ -3166,7 +3166,7 @@
     </cx:data>
     <cx:data id="14">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4195,17 +4195,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.40</cx:f>
+        <cx:f>_xlchart.v1.36</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.42</cx:f>
+        <cx:f>_xlchart.v1.38</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.44</cx:f>
+        <cx:f>_xlchart.v1.40</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4276,7 +4276,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24BF4607-F4E8-E345-97F3-975C8A945A06}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.39</cx:f>
+              <cx:f>_xlchart.v1.35</cx:f>
               <cx:v>rcp26</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4289,7 +4289,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B15400F1-0218-BE43-9F95-AD4EAABB47CD}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.41</cx:f>
+              <cx:f>_xlchart.v1.37</cx:f>
               <cx:v>rcp45</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4302,7 +4302,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{99A6A248-8D06-4B4A-861B-9E311114F9A0}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.43</cx:f>
+              <cx:f>_xlchart.v1.39</cx:f>
               <cx:v>rcp85</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4368,22 +4368,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.35</cx:f>
+        <cx:f>_xlchart.v1.41</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.36</cx:f>
+        <cx:f>_xlchart.v1.42</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.37</cx:f>
+        <cx:f>_xlchart.v1.43</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.38</cx:f>
+        <cx:f>_xlchart.v1.44</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8666,7 +8666,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{046980F5-1704-F8BB-6927-DBD6B2746A1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{318E6868-8130-118B-A1D7-A96E632B99EF}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -8777,7 +8777,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25624F71-0E2B-E1CB-44FC-0C6A7492A11E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D515273-EE15-C455-5F45-AC20FC867064}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -8888,7 +8888,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B8A96AD-7BB9-36D1-5BC9-7A4194A42716}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C463DE76-C613-AE6A-0441-1161334F9CC4}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -9611,6 +9611,12 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3"/>
+          <cell r="K3"/>
+          <cell r="L3"/>
+          <cell r="M3"/>
+        </row>
         <row r="4">
           <cell r="B4">
             <v>2068</v>
@@ -9618,6 +9624,9 @@
           <cell r="J4">
             <v>0.953297643723377</v>
           </cell>
+          <cell r="K4"/>
+          <cell r="L4"/>
+          <cell r="M4"/>
         </row>
         <row r="5">
           <cell r="B5">
@@ -9632,6 +9641,8 @@
           <cell r="K5">
             <v>1.12528774120191</v>
           </cell>
+          <cell r="L5"/>
+          <cell r="M5"/>
         </row>
         <row r="6">
           <cell r="B6">
@@ -9640,6 +9651,9 @@
           <cell r="J6">
             <v>0.962655414052216</v>
           </cell>
+          <cell r="K6"/>
+          <cell r="L6"/>
+          <cell r="M6"/>
         </row>
         <row r="7">
           <cell r="B7">
@@ -9654,6 +9668,20 @@
           <cell r="K7">
             <v>0.75275346345142902</v>
           </cell>
+          <cell r="L7"/>
+          <cell r="M7"/>
+        </row>
+        <row r="8">
+          <cell r="J8"/>
+          <cell r="K8"/>
+          <cell r="L8"/>
+          <cell r="M8"/>
+        </row>
+        <row r="9">
+          <cell r="J9"/>
+          <cell r="K9"/>
+          <cell r="L9"/>
+          <cell r="M9"/>
         </row>
         <row r="10">
           <cell r="B10">
@@ -9668,6 +9696,26 @@
           <cell r="K10">
             <v>1.2996490999999999</v>
           </cell>
+          <cell r="L10"/>
+          <cell r="M10"/>
+        </row>
+        <row r="11">
+          <cell r="J11"/>
+          <cell r="K11"/>
+          <cell r="L11"/>
+          <cell r="M11"/>
+        </row>
+        <row r="12">
+          <cell r="J12"/>
+          <cell r="K12"/>
+          <cell r="L12"/>
+          <cell r="M12"/>
+        </row>
+        <row r="13">
+          <cell r="J13"/>
+          <cell r="K13"/>
+          <cell r="L13"/>
+          <cell r="M13"/>
         </row>
         <row r="14">
           <cell r="B14">
@@ -9676,6 +9724,9 @@
           <cell r="J14">
             <v>1.1676970687033701</v>
           </cell>
+          <cell r="K14"/>
+          <cell r="L14"/>
+          <cell r="M14"/>
         </row>
         <row r="15">
           <cell r="B15">
@@ -9690,6 +9741,8 @@
           <cell r="K15">
             <v>2.1459751510413598</v>
           </cell>
+          <cell r="L15"/>
+          <cell r="M15"/>
         </row>
         <row r="16">
           <cell r="B16">
@@ -9704,6 +9757,8 @@
           <cell r="K16">
             <v>1.8127139886377099</v>
           </cell>
+          <cell r="L16"/>
+          <cell r="M16"/>
         </row>
         <row r="17">
           <cell r="B17">
@@ -9718,6 +9773,8 @@
           <cell r="K17">
             <v>1.8433555303092599</v>
           </cell>
+          <cell r="L17"/>
+          <cell r="M17"/>
         </row>
         <row r="18">
           <cell r="B18">
@@ -9732,6 +9789,8 @@
           <cell r="K18">
             <v>1.2746751758441699</v>
           </cell>
+          <cell r="L18"/>
+          <cell r="M18"/>
         </row>
         <row r="19">
           <cell r="B19">
@@ -9740,6 +9799,15 @@
           <cell r="J19">
             <v>0.50765736677745898</v>
           </cell>
+          <cell r="K19"/>
+          <cell r="L19"/>
+          <cell r="M19"/>
+        </row>
+        <row r="20">
+          <cell r="J20"/>
+          <cell r="K20"/>
+          <cell r="L20"/>
+          <cell r="M20"/>
         </row>
         <row r="21">
           <cell r="B21">
@@ -9754,6 +9822,8 @@
           <cell r="K21">
             <v>3.1213066025999701</v>
           </cell>
+          <cell r="L21"/>
+          <cell r="M21"/>
         </row>
         <row r="22">
           <cell r="B22">
@@ -9768,6 +9838,8 @@
           <cell r="K22">
             <v>1.3981454217936999</v>
           </cell>
+          <cell r="L22"/>
+          <cell r="M22"/>
         </row>
         <row r="23">
           <cell r="B23">
@@ -9782,6 +9854,8 @@
           <cell r="K23">
             <v>1.67016129100406</v>
           </cell>
+          <cell r="L23"/>
+          <cell r="M23"/>
         </row>
         <row r="24">
           <cell r="B24">
@@ -9796,6 +9870,8 @@
           <cell r="K24">
             <v>1.0728179942746401</v>
           </cell>
+          <cell r="L24"/>
+          <cell r="M24"/>
         </row>
         <row r="25">
           <cell r="B25">
@@ -9810,6 +9886,8 @@
           <cell r="K25">
             <v>1.6734034587411499</v>
           </cell>
+          <cell r="L25"/>
+          <cell r="M25"/>
         </row>
         <row r="26">
           <cell r="B26">
@@ -9824,6 +9902,8 @@
           <cell r="K26">
             <v>0.94311847540844496</v>
           </cell>
+          <cell r="L26"/>
+          <cell r="M26"/>
         </row>
         <row r="27">
           <cell r="B27">
@@ -9838,6 +9918,8 @@
           <cell r="K27">
             <v>1.4934826904101901</v>
           </cell>
+          <cell r="L27"/>
+          <cell r="M27"/>
         </row>
         <row r="28">
           <cell r="B28">
@@ -9846,6 +9928,9 @@
           <cell r="J28">
             <v>1.0283560461610499</v>
           </cell>
+          <cell r="K28"/>
+          <cell r="L28"/>
+          <cell r="M28"/>
         </row>
         <row r="29">
           <cell r="B29">
@@ -9860,6 +9945,8 @@
           <cell r="K29">
             <v>0.45363177546752198</v>
           </cell>
+          <cell r="L29"/>
+          <cell r="M29"/>
         </row>
         <row r="30">
           <cell r="B30">
@@ -9874,6 +9961,8 @@
           <cell r="K30">
             <v>0.91811225325973</v>
           </cell>
+          <cell r="L30"/>
+          <cell r="M30"/>
         </row>
         <row r="31">
           <cell r="B31">
@@ -9882,6 +9971,9 @@
           <cell r="J31">
             <v>1.0129333473675</v>
           </cell>
+          <cell r="K31"/>
+          <cell r="L31"/>
+          <cell r="M31"/>
         </row>
         <row r="32">
           <cell r="B32">
@@ -9896,6 +9988,8 @@
           <cell r="K32">
             <v>0.93398420658576498</v>
           </cell>
+          <cell r="L32"/>
+          <cell r="M32"/>
         </row>
         <row r="33">
           <cell r="B33">
@@ -9910,6 +10004,8 @@
           <cell r="K33">
             <v>1.9070619275280301</v>
           </cell>
+          <cell r="L33"/>
+          <cell r="M33"/>
         </row>
         <row r="34">
           <cell r="B34">
@@ -9924,6 +10020,14 @@
           <cell r="K34">
             <v>1.03584774279575</v>
           </cell>
+          <cell r="L34"/>
+          <cell r="M34"/>
+        </row>
+        <row r="35">
+          <cell r="J35"/>
+          <cell r="K35"/>
+          <cell r="L35"/>
+          <cell r="M35"/>
         </row>
         <row r="36">
           <cell r="B36">
@@ -9938,6 +10042,14 @@
           <cell r="K36">
             <v>1.1211079653474301</v>
           </cell>
+          <cell r="L36"/>
+          <cell r="M36"/>
+        </row>
+        <row r="37">
+          <cell r="J37"/>
+          <cell r="K37"/>
+          <cell r="L37"/>
+          <cell r="M37"/>
         </row>
         <row r="38">
           <cell r="B38">
@@ -9946,6 +10058,9 @@
           <cell r="J38">
             <v>1.47924744842162</v>
           </cell>
+          <cell r="K38"/>
+          <cell r="L38"/>
+          <cell r="M38"/>
         </row>
         <row r="39">
           <cell r="B39">
@@ -9960,6 +10075,8 @@
           <cell r="K39">
             <v>1.47625627991256</v>
           </cell>
+          <cell r="L39"/>
+          <cell r="M39"/>
         </row>
         <row r="40">
           <cell r="B40">
@@ -9974,6 +10091,8 @@
           <cell r="K40">
             <v>1.22094780806839</v>
           </cell>
+          <cell r="L40"/>
+          <cell r="M40"/>
         </row>
         <row r="41">
           <cell r="B41">
@@ -9988,6 +10107,8 @@
           <cell r="K41">
             <v>1.7052057166927399</v>
           </cell>
+          <cell r="L41"/>
+          <cell r="M41"/>
         </row>
         <row r="42">
           <cell r="B42">
@@ -9996,6 +10117,9 @@
           <cell r="J42">
             <v>0.81285915249012197</v>
           </cell>
+          <cell r="K42"/>
+          <cell r="L42"/>
+          <cell r="M42"/>
         </row>
         <row r="43">
           <cell r="B43">
@@ -10004,6 +10128,9 @@
           <cell r="J43">
             <v>0.85479150373844803</v>
           </cell>
+          <cell r="K43"/>
+          <cell r="L43"/>
+          <cell r="M43"/>
         </row>
         <row r="44">
           <cell r="B44">
@@ -10012,6 +10139,9 @@
           <cell r="J44">
             <v>1.24668562684192</v>
           </cell>
+          <cell r="K44"/>
+          <cell r="L44"/>
+          <cell r="M44"/>
         </row>
         <row r="45">
           <cell r="B45">
@@ -10052,6 +10182,8 @@
           <cell r="K46">
             <v>0.99413149999999995</v>
           </cell>
+          <cell r="L46"/>
+          <cell r="M46"/>
         </row>
         <row r="47">
           <cell r="B47">
@@ -10066,6 +10198,8 @@
           <cell r="K47">
             <v>1.2139563001517599</v>
           </cell>
+          <cell r="L47"/>
+          <cell r="M47"/>
         </row>
         <row r="48">
           <cell r="B48">
@@ -10074,6 +10208,9 @@
           <cell r="J48">
             <v>0.31548891067506302</v>
           </cell>
+          <cell r="K48"/>
+          <cell r="L48"/>
+          <cell r="M48"/>
         </row>
         <row r="49">
           <cell r="B49">
@@ -10088,6 +10225,8 @@
           <cell r="K49">
             <v>1.43005460103351</v>
           </cell>
+          <cell r="L49"/>
+          <cell r="M49"/>
         </row>
         <row r="50">
           <cell r="B50">
@@ -10096,6 +10235,9 @@
           <cell r="J50">
             <v>1.58398556179473</v>
           </cell>
+          <cell r="K50"/>
+          <cell r="L50"/>
+          <cell r="M50"/>
         </row>
         <row r="51">
           <cell r="B51">
@@ -10104,6 +10246,9 @@
           <cell r="J51">
             <v>1.5601286800869001</v>
           </cell>
+          <cell r="K51"/>
+          <cell r="L51"/>
+          <cell r="M51"/>
         </row>
         <row r="52">
           <cell r="B52">
@@ -10112,6 +10257,9 @@
           <cell r="J52">
             <v>0.89465247498328804</v>
           </cell>
+          <cell r="K52"/>
+          <cell r="L52"/>
+          <cell r="M52"/>
         </row>
         <row r="53">
           <cell r="B53">
@@ -10120,6 +10268,9 @@
           <cell r="J53">
             <v>1.4470739576551801</v>
           </cell>
+          <cell r="K53"/>
+          <cell r="L53"/>
+          <cell r="M53"/>
         </row>
         <row r="54">
           <cell r="B54">
@@ -10128,6 +10279,9 @@
           <cell r="J54">
             <v>0.93532776547523599</v>
           </cell>
+          <cell r="K54"/>
+          <cell r="L54"/>
+          <cell r="M54"/>
         </row>
         <row r="55">
           <cell r="B55">
@@ -10142,6 +10296,20 @@
           <cell r="K55">
             <v>1.4829433865017501</v>
           </cell>
+          <cell r="L55"/>
+          <cell r="M55"/>
+        </row>
+        <row r="56">
+          <cell r="J56"/>
+          <cell r="K56"/>
+          <cell r="L56"/>
+          <cell r="M56"/>
+        </row>
+        <row r="57">
+          <cell r="J57"/>
+          <cell r="K57"/>
+          <cell r="L57"/>
+          <cell r="M57"/>
         </row>
         <row r="58">
           <cell r="B58">
@@ -10156,6 +10324,8 @@
           <cell r="K58">
             <v>1.7895930232263599</v>
           </cell>
+          <cell r="L58"/>
+          <cell r="M58"/>
         </row>
         <row r="59">
           <cell r="B59">
@@ -10170,6 +10340,8 @@
           <cell r="K59">
             <v>1.8116578232415801</v>
           </cell>
+          <cell r="L59"/>
+          <cell r="M59"/>
         </row>
         <row r="60">
           <cell r="B60">
@@ -10190,6 +10362,7 @@
           <cell r="L60">
             <v>3.0059425348697002</v>
           </cell>
+          <cell r="M60"/>
         </row>
         <row r="61">
           <cell r="B61">
@@ -10204,6 +10377,8 @@
           <cell r="K61">
             <v>1.7521867119608101</v>
           </cell>
+          <cell r="L61"/>
+          <cell r="M61"/>
         </row>
         <row r="62">
           <cell r="B62">
@@ -10218,6 +10393,8 @@
           <cell r="K62">
             <v>1.1976161575342901</v>
           </cell>
+          <cell r="L62"/>
+          <cell r="M62"/>
         </row>
         <row r="63">
           <cell r="B63">
@@ -10232,6 +10409,8 @@
           <cell r="K63">
             <v>1.79025508687392</v>
           </cell>
+          <cell r="L63"/>
+          <cell r="M63"/>
         </row>
         <row r="64">
           <cell r="B64">
@@ -10246,6 +10425,8 @@
           <cell r="K64">
             <v>1.8836058328781899</v>
           </cell>
+          <cell r="L64"/>
+          <cell r="M64"/>
         </row>
         <row r="65">
           <cell r="B65">
@@ -10266,6 +10447,7 @@
           <cell r="L65">
             <v>4.2916051539023199</v>
           </cell>
+          <cell r="M65"/>
         </row>
         <row r="66">
           <cell r="B66">
@@ -10286,6 +10468,7 @@
           <cell r="L66">
             <v>2.0659365442925499</v>
           </cell>
+          <cell r="M66"/>
         </row>
         <row r="67">
           <cell r="B67">
@@ -10306,6 +10489,7 @@
           <cell r="L67">
             <v>2.07600407171268</v>
           </cell>
+          <cell r="M67"/>
         </row>
         <row r="68">
           <cell r="B68">
@@ -10326,6 +10510,7 @@
           <cell r="L68">
             <v>2.46145115976516</v>
           </cell>
+          <cell r="M68"/>
         </row>
         <row r="69">
           <cell r="B69">
@@ -10346,6 +10531,7 @@
           <cell r="L69">
             <v>2.95128872598479</v>
           </cell>
+          <cell r="M69"/>
         </row>
         <row r="70">
           <cell r="B70">
@@ -10366,6 +10552,7 @@
           <cell r="L70">
             <v>2.4659900553596299</v>
           </cell>
+          <cell r="M70"/>
         </row>
         <row r="71">
           <cell r="B71">
@@ -10386,6 +10573,7 @@
           <cell r="L71">
             <v>1.9276448337221399</v>
           </cell>
+          <cell r="M71"/>
         </row>
         <row r="72">
           <cell r="B72">
@@ -10406,6 +10594,7 @@
           <cell r="L72">
             <v>2.2183875868211</v>
           </cell>
+          <cell r="M72"/>
         </row>
         <row r="73">
           <cell r="B73">
@@ -10478,6 +10667,7 @@
           <cell r="L75">
             <v>1.7990900046379901</v>
           </cell>
+          <cell r="M75"/>
         </row>
         <row r="76">
           <cell r="B76">
@@ -10498,6 +10688,7 @@
           <cell r="L76">
             <v>2.3771028757036698</v>
           </cell>
+          <cell r="M76"/>
         </row>
         <row r="77">
           <cell r="B77">
@@ -10518,6 +10709,7 @@
           <cell r="L77">
             <v>1.64459827038435</v>
           </cell>
+          <cell r="M77"/>
         </row>
         <row r="78">
           <cell r="B78">
@@ -10538,6 +10730,7 @@
           <cell r="L78">
             <v>2.4737583558019298</v>
           </cell>
+          <cell r="M78"/>
         </row>
         <row r="79">
           <cell r="B79">
@@ -10552,6 +10745,8 @@
           <cell r="K79">
             <v>1.1256945521228801</v>
           </cell>
+          <cell r="L79"/>
+          <cell r="M79"/>
         </row>
         <row r="80">
           <cell r="B80">
@@ -10566,6 +10761,8 @@
           <cell r="K80">
             <v>1.42677008310954</v>
           </cell>
+          <cell r="L80"/>
+          <cell r="M80"/>
         </row>
         <row r="81">
           <cell r="B81">
@@ -10586,6 +10783,7 @@
           <cell r="L81">
             <v>2.1591106380818599</v>
           </cell>
+          <cell r="M81"/>
         </row>
         <row r="82">
           <cell r="B82">
@@ -10600,6 +10798,8 @@
           <cell r="K82">
             <v>1.6772889300680101</v>
           </cell>
+          <cell r="L82"/>
+          <cell r="M82"/>
         </row>
         <row r="83">
           <cell r="B83">
@@ -10614,6 +10814,8 @@
           <cell r="K83">
             <v>1.65557634817044</v>
           </cell>
+          <cell r="L83"/>
+          <cell r="M83"/>
         </row>
         <row r="84">
           <cell r="B84">
@@ -10628,6 +10830,8 @@
           <cell r="K84">
             <v>1.79784619645486</v>
           </cell>
+          <cell r="L84"/>
+          <cell r="M84"/>
         </row>
         <row r="85">
           <cell r="B85">
@@ -10642,6 +10846,8 @@
           <cell r="K85">
             <v>1.7099448768059999</v>
           </cell>
+          <cell r="L85"/>
+          <cell r="M85"/>
         </row>
         <row r="86">
           <cell r="B86">
@@ -10662,6 +10868,7 @@
           <cell r="L86">
             <v>2.7137934503127701</v>
           </cell>
+          <cell r="M86"/>
         </row>
         <row r="87">
           <cell r="B87">
@@ -10682,6 +10889,7 @@
           <cell r="L87">
             <v>2.6473017385885602</v>
           </cell>
+          <cell r="M87"/>
         </row>
         <row r="88">
           <cell r="B88">
@@ -10696,6 +10904,8 @@
           <cell r="K88">
             <v>1.4064785184664499</v>
           </cell>
+          <cell r="L88"/>
+          <cell r="M88"/>
         </row>
         <row r="89">
           <cell r="B89">
@@ -10710,6 +10920,8 @@
           <cell r="K89">
             <v>1.8829193396530901</v>
           </cell>
+          <cell r="L89"/>
+          <cell r="M89"/>
         </row>
         <row r="90">
           <cell r="B90">
@@ -10724,6 +10936,8 @@
           <cell r="K90">
             <v>1.9885308508852599</v>
           </cell>
+          <cell r="L90"/>
+          <cell r="M90"/>
         </row>
         <row r="91">
           <cell r="B91">
@@ -10744,6 +10958,7 @@
           <cell r="L91">
             <v>2.7629134999999998</v>
           </cell>
+          <cell r="M91"/>
         </row>
         <row r="92">
           <cell r="B92">
@@ -10764,6 +10979,7 @@
           <cell r="L92">
             <v>2.61799366766664</v>
           </cell>
+          <cell r="M92"/>
         </row>
         <row r="93">
           <cell r="B93">
@@ -10778,6 +10994,8 @@
           <cell r="K93">
             <v>0.74702986611260902</v>
           </cell>
+          <cell r="L93"/>
+          <cell r="M93"/>
         </row>
         <row r="94">
           <cell r="B94">
@@ -10792,6 +11010,8 @@
           <cell r="K94">
             <v>1.81199906667073</v>
           </cell>
+          <cell r="L94"/>
+          <cell r="M94"/>
         </row>
         <row r="95">
           <cell r="B95">
@@ -10806,6 +11026,8 @@
           <cell r="K95">
             <v>2.3510983361137998</v>
           </cell>
+          <cell r="L95"/>
+          <cell r="M95"/>
         </row>
         <row r="96">
           <cell r="B96">
@@ -10820,6 +11042,8 @@
           <cell r="K96">
             <v>1.8110792384853101</v>
           </cell>
+          <cell r="L96"/>
+          <cell r="M96"/>
         </row>
         <row r="97">
           <cell r="B97">
@@ -10834,6 +11058,8 @@
           <cell r="K97">
             <v>1.5849269976389799</v>
           </cell>
+          <cell r="L97"/>
+          <cell r="M97"/>
         </row>
         <row r="98">
           <cell r="B98">
@@ -10848,6 +11074,8 @@
           <cell r="K98">
             <v>1.61900668674048</v>
           </cell>
+          <cell r="L98"/>
+          <cell r="M98"/>
         </row>
         <row r="99">
           <cell r="B99">
@@ -10862,6 +11090,8 @@
           <cell r="K99">
             <v>1.3695843568142401</v>
           </cell>
+          <cell r="L99"/>
+          <cell r="M99"/>
         </row>
         <row r="100">
           <cell r="B100">
@@ -10876,6 +11106,8 @@
           <cell r="K100">
             <v>1.71808351940573</v>
           </cell>
+          <cell r="L100"/>
+          <cell r="M100"/>
         </row>
         <row r="101">
           <cell r="B101">
@@ -10890,6 +11122,8 @@
           <cell r="K101">
             <v>2.1603128362584698</v>
           </cell>
+          <cell r="L101"/>
+          <cell r="M101"/>
         </row>
         <row r="102">
           <cell r="B102">
@@ -10904,6 +11138,8 @@
           <cell r="K102">
             <v>1.9302608195684401</v>
           </cell>
+          <cell r="L102"/>
+          <cell r="M102"/>
         </row>
         <row r="103">
           <cell r="B103">
@@ -10924,6 +11160,7 @@
           <cell r="L103">
             <v>3.1708323798723201</v>
           </cell>
+          <cell r="M103"/>
         </row>
         <row r="104">
           <cell r="B104">
@@ -10996,6 +11233,7 @@
           <cell r="L106">
             <v>3.02139535831243</v>
           </cell>
+          <cell r="M106"/>
         </row>
         <row r="107">
           <cell r="B107">
@@ -11016,6 +11254,7 @@
           <cell r="L107">
             <v>2.7878231845461698</v>
           </cell>
+          <cell r="M107"/>
         </row>
         <row r="108">
           <cell r="B108">
@@ -11036,6 +11275,7 @@
           <cell r="L108">
             <v>3.1576496725510599</v>
           </cell>
+          <cell r="M108"/>
         </row>
         <row r="109">
           <cell r="B109">
@@ -11044,6 +11284,9 @@
           <cell r="J109">
             <v>1.5657428882740401</v>
           </cell>
+          <cell r="K109"/>
+          <cell r="L109"/>
+          <cell r="M109"/>
         </row>
         <row r="110">
           <cell r="B110">
@@ -11058,6 +11301,8 @@
           <cell r="K110">
             <v>1.8104741339919299</v>
           </cell>
+          <cell r="L110"/>
+          <cell r="M110"/>
         </row>
         <row r="111">
           <cell r="B111">
@@ -11078,6 +11323,7 @@
           <cell r="L111">
             <v>4.1255501015432303</v>
           </cell>
+          <cell r="M111"/>
         </row>
         <row r="112">
           <cell r="B112">
@@ -11436,6 +11682,7 @@
           <cell r="L125">
             <v>2.1705614599349499</v>
           </cell>
+          <cell r="M125"/>
         </row>
         <row r="126">
           <cell r="B126">
@@ -11456,6 +11703,7 @@
           <cell r="L126">
             <v>2.21875868903268</v>
           </cell>
+          <cell r="M126"/>
         </row>
         <row r="127">
           <cell r="B127">
@@ -11476,6 +11724,7 @@
           <cell r="L127">
             <v>3.0087400281739001</v>
           </cell>
+          <cell r="M127"/>
         </row>
         <row r="128">
           <cell r="B128">
@@ -11496,6 +11745,7 @@
           <cell r="L128">
             <v>2.5273760401932899</v>
           </cell>
+          <cell r="M128"/>
         </row>
         <row r="129">
           <cell r="B129">
@@ -11516,6 +11766,7 @@
           <cell r="L129">
             <v>2.6335885440636302</v>
           </cell>
+          <cell r="M129"/>
         </row>
         <row r="130">
           <cell r="B130">
@@ -11536,6 +11787,7 @@
           <cell r="L130">
             <v>2.3055320339923799</v>
           </cell>
+          <cell r="M130"/>
         </row>
         <row r="131">
           <cell r="B131">
@@ -11556,6 +11808,7 @@
           <cell r="L131">
             <v>2.8297057592542201</v>
           </cell>
+          <cell r="M131"/>
         </row>
         <row r="132">
           <cell r="B132">
@@ -11576,6 +11829,7 @@
           <cell r="L132">
             <v>3.20905435545248</v>
           </cell>
+          <cell r="M132"/>
         </row>
         <row r="133">
           <cell r="B133">
@@ -11674,6 +11928,7 @@
           <cell r="L136">
             <v>2.4212512758043401</v>
           </cell>
+          <cell r="M136"/>
         </row>
         <row r="137">
           <cell r="B137">
@@ -11694,6 +11949,7 @@
           <cell r="L137">
             <v>3.4698040573684898</v>
           </cell>
+          <cell r="M137"/>
         </row>
         <row r="138">
           <cell r="B138">
@@ -11708,6 +11964,8 @@
           <cell r="K138">
             <v>2.2215974851091702</v>
           </cell>
+          <cell r="L138"/>
+          <cell r="M138"/>
         </row>
         <row r="139">
           <cell r="B139">
@@ -11716,6 +11974,9 @@
           <cell r="J139">
             <v>1.4871546851264099</v>
           </cell>
+          <cell r="K139"/>
+          <cell r="L139"/>
+          <cell r="M139"/>
         </row>
         <row r="140">
           <cell r="B140">
@@ -11736,6 +11997,7 @@
           <cell r="L140">
             <v>2.76461721959198</v>
           </cell>
+          <cell r="M140"/>
         </row>
         <row r="141">
           <cell r="B141">
@@ -11756,6 +12018,7 @@
           <cell r="L141">
             <v>3.0094896104601001</v>
           </cell>
+          <cell r="M141"/>
         </row>
         <row r="142">
           <cell r="B142">
@@ -11776,6 +12039,7 @@
           <cell r="L142">
             <v>2.2740586286362601</v>
           </cell>
+          <cell r="M142"/>
         </row>
         <row r="143">
           <cell r="B143">
@@ -11790,6 +12054,8 @@
           <cell r="K143">
             <v>2.1390993330213699</v>
           </cell>
+          <cell r="L143"/>
+          <cell r="M143"/>
         </row>
         <row r="144">
           <cell r="B144">
@@ -11810,6 +12076,7 @@
           <cell r="L144">
             <v>3.6687247613706999</v>
           </cell>
+          <cell r="M144"/>
         </row>
         <row r="145">
           <cell r="B145">
@@ -11960,6 +12227,7 @@
           <cell r="L150">
             <v>3.30951525175441</v>
           </cell>
+          <cell r="M150"/>
         </row>
         <row r="151">
           <cell r="B151">
@@ -11980,6 +12248,7 @@
           <cell r="L151">
             <v>2.9504145044591001</v>
           </cell>
+          <cell r="M151"/>
         </row>
         <row r="152">
           <cell r="B152">
@@ -12390,6 +12659,7 @@
           <cell r="L167">
             <v>2.2516428417629699</v>
           </cell>
+          <cell r="M167"/>
         </row>
         <row r="168">
           <cell r="B168">
@@ -12488,6 +12758,7 @@
           <cell r="L171">
             <v>3.04848111038363</v>
           </cell>
+          <cell r="M171"/>
         </row>
         <row r="172">
           <cell r="B172">
@@ -12586,6 +12857,7 @@
           <cell r="L175">
             <v>2.5286943670620601</v>
           </cell>
+          <cell r="M175"/>
         </row>
         <row r="176">
           <cell r="B176">
@@ -12606,6 +12878,7 @@
           <cell r="L176">
             <v>2.7677175902520599</v>
           </cell>
+          <cell r="M176"/>
         </row>
         <row r="177">
           <cell r="B177">
@@ -12626,6 +12899,7 @@
           <cell r="L177">
             <v>2.9216101985538199</v>
           </cell>
+          <cell r="M177"/>
         </row>
         <row r="178">
           <cell r="B178">
@@ -12698,6 +12972,7 @@
           <cell r="L180">
             <v>2.3987316555447</v>
           </cell>
+          <cell r="M180"/>
         </row>
         <row r="181">
           <cell r="B181">
@@ -12744,6 +13019,7 @@
           <cell r="L182">
             <v>3.49936630814164</v>
           </cell>
+          <cell r="M182"/>
         </row>
         <row r="183">
           <cell r="B183">
@@ -12764,6 +13040,7 @@
           <cell r="L183">
             <v>3.3262258100273101</v>
           </cell>
+          <cell r="M183"/>
         </row>
         <row r="184">
           <cell r="B184">
@@ -12784,6 +13061,7 @@
           <cell r="L184">
             <v>2.8145093766053302</v>
           </cell>
+          <cell r="M184"/>
         </row>
         <row r="185">
           <cell r="B185">
@@ -12804,6 +13082,7 @@
           <cell r="L185">
             <v>2.8472741021049801</v>
           </cell>
+          <cell r="M185"/>
         </row>
         <row r="186">
           <cell r="B186">
@@ -12876,6 +13155,7 @@
           <cell r="L188">
             <v>3.3017069074842902</v>
           </cell>
+          <cell r="M188"/>
         </row>
         <row r="189">
           <cell r="B189">
@@ -12896,6 +13176,7 @@
           <cell r="L189">
             <v>3.3375443506061302</v>
           </cell>
+          <cell r="M189"/>
         </row>
         <row r="190">
           <cell r="B190">
@@ -13255,7 +13536,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13729,7 +14010,7 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14697,6 +14978,7 @@
         <v>1.7608200000000001</v>
       </c>
       <c r="R25" s="3"/>
+      <c r="W25" s="3"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
Updated GWL calculation to CMIP6 and added indicator scripts
</commit_message>
<xml_diff>
--- a/data/gwl_lists/GWLs_CMIP5_OEKS15.xlsx
+++ b/data/gwl_lists/GWLs_CMIP5_OEKS15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbecsi/Desktop/Arbeit/Qgis/data/AAR2/GWLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A90744A-6723-1446-81D3-A072BC41B0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F077F4C1-3AA2-6E43-9657-A1CE066C45AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22120" activeTab="1" xr2:uid="{B7CF2435-4AB2-8449-A283-99C1C1B4CF66}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22120" activeTab="4" xr2:uid="{B7CF2435-4AB2-8449-A283-99C1C1B4CF66}"/>
   </bookViews>
   <sheets>
     <sheet name="lookup_table" sheetId="8" r:id="rId1"/>
@@ -32,42 +32,46 @@
     <definedName name="_xlchart.v1.1" hidden="1">[1]Tabelle2!$C$3:$C$27</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">Tabelle2!$E$3:$E$33</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Tabelle2!$F$3:$F$33</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">[1]Tabelle2!$B$12:$B$19</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">[1]Tabelle2!$B$20:$B$27</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">[1]Tabelle2!$B$3:$B$11</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">[1]Tabelle2!$C$12:$C$19</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">[1]Tabelle2!$C$20:$C$27</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">[1]Tabelle2!$C$3:$C$11</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">[1]Tabelle2!$F$33:$F$42</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">[1]Tabelle2!$J$3:$J$27</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">[1]Tabelle2!$B$3:$B$27</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">[1]Tabelle2!$C$3:$C$27</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">[1]Tabelle2!$D$3:$D$27</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">[1]Tabelle2!$E$3:$E$27</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">[2]Tabelle2!$B$3:$B$191</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">[2]Tabelle2!$C$3:$C$191</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">[2]Tabelle2!$D$3:$D$191</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">[2]Tabelle2!$E$3:$E$191</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">[1]Tabelle2!$D$3:$D$27</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">[1]Tabelle2!$K$3:$K$27</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">[1]Tabelle2!$L$3:$L$27</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">[1]Tabelle2!$M$3:$M$27</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">[2]Tabelle2!$J$3:$J$191</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">[2]Tabelle2!$K$3:$K$191</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">[2]Tabelle2!$L$3:$L$191</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">[2]Tabelle2!$M$3:$M$191</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">[1]Tabelle2!$J$3:$J$27</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">[1]Tabelle2!$K$3:$K$27</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">[1]Tabelle2!$L$3:$L$27</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Tabelle2!$C$3:$C$33</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Tabelle2!$D$3:$D$33</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Tabelle2!$E$3:$E$33</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Tabelle2!$F$3:$F$33</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">[1]Tabelle2!$B$12:$B$19</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">[1]Tabelle2!$B$20:$B$27</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">[1]Tabelle2!$B$3:$B$11</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">[1]Tabelle2!$C$12:$C$19</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">[1]Tabelle2!$C$20:$C$27</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">[1]Tabelle2!$C$3:$C$11</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">[1]Tabelle2!$E$3:$E$27</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">[1]Tabelle2!$M$3:$M$27</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">[2]Tabelle2!$J$3:$J$191</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">[2]Tabelle2!$K$3:$K$191</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">[2]Tabelle2!$L$3:$L$191</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">[2]Tabelle2!$M$3:$M$191</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Tabelle1!$D$2</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Tabelle1!$D$3:$D$15</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Tabelle1!$E$2</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Tabelle1!$E$3:$E$15</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Tabelle1!$F$2</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">[1]Tabelle2!$F$33:$F$42</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">[1]Tabelle2!$J$3:$J$27</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">[1]Tabelle2!$K$3:$K$27</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">[1]Tabelle2!$L$3:$L$27</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">[1]Tabelle2!$M$3:$M$27</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">[2]Tabelle2!$J$3:$J$191</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">[2]Tabelle2!$K$3:$K$191</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">[2]Tabelle2!$L$3:$L$191</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">[2]Tabelle2!$M$3:$M$191</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Tabelle1!$G$3:$G$36</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">[2]Tabelle2!$B$3:$B$191</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Tabelle1!$F$3:$F$15</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Tabelle1!$G$3:$G$36</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Tabelle1!$H$3:$H$36</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Tabelle1!$I$3:$I$36</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Tabelle1!$J$3:$J$36</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Tabelle1!$H$3:$H$36</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Tabelle1!$I$3:$I$36</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Tabelle1!$J$3:$J$36</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Tabelle1!$D$2</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Tabelle1!$D$3:$D$15</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">Tabelle1!$E$2</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Tabelle1!$E$3:$E$15</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">Tabelle1!$F$2</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">Tabelle1!$F$3:$F$15</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">[2]Tabelle2!$C$3:$C$191</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">[2]Tabelle2!$D$3:$D$191</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">[2]Tabelle2!$E$3:$E$191</definedName>
@@ -522,7 +526,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,6 +542,90 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -625,6 +713,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2182,7 +2284,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2195,9 +2297,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1600"/>
-              <a:t>CCS AUT CMIP5 vs. ÖKS15</a:t>
+              <a:rPr lang="de-DE" sz="1400" b="1"/>
+              <a:t>Temperature</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="1" baseline="0"/>
+              <a:t> signals of OEKS15 models vs. GCM background models for all GWLs</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="1400" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2205,8 +2312,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.36209711286089241"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.15607556854496674"/>
+          <c:y val="4.2527140032163381E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2222,7 +2329,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2245,10 +2352,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.7319853392490752E-2"/>
-          <c:y val="0.11378196282165759"/>
-          <c:w val="0.90202321870122582"/>
-          <c:h val="0.81273016130715614"/>
+          <c:x val="9.3045102087654485E-2"/>
+          <c:y val="0.13695966934728043"/>
+          <c:w val="0.88293696330744209"/>
+          <c:h val="0.74530419748244281"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2295,6 +2402,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.1273561765386219E-3"/>
+                  <c:y val="-2.8291533046607042E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2308,7 +2421,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -2852,7 +2965,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.5"/>
-          <c:min val="-0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2877,11 +2989,24 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1200"/>
-                  <a:t>CCS AUT from CMIP5 GCM</a:t>
+                  <a:t>Temperature</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200" baseline="0"/>
+                  <a:t> signal (vs. 1991-2020) of CMIP5 GCMs</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.34416939631084215"/>
+              <c:y val="0.94708073248098545"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2912,7 +3037,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -2933,7 +3058,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2956,7 +3081,6 @@
         <c:axId val="2049064480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2981,11 +3105,24 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1200"/>
-                  <a:t>CCS AUT from OEKS15</a:t>
+                  <a:t>Temperature</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200" baseline="0"/>
+                  <a:t> signal (vs. 1991-2020) of OEKS15 models</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.3277052246216088E-2"/>
+              <c:y val="0.22671236501740155"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3037,7 +3174,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3059,7 +3196,9 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:srgbClr val="DADADA"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -3108,65 +3247,65 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3"/>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7"/>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.18</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11"/>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="14">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3174,7 +3313,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Date of reaching GWL: CMIP5 (ÖKS15) vs. CMIP5 (whole ensemble) vs. CMIP6</cx:v>
+          <cx:v>Date of reaching GWLs: CMIP5 (OEKS15) vs. CMIP5 (whole ensemble) vs. CMIP6</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -3182,10 +3321,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
+            <a:defRPr b="1"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="de-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -3194,18 +3333,26 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Date of reaching GWL: CMIP5 (ÖKS15) vs. CMIP5 (whole ensemble) vs. CMIP6</a:t>
+            <a:t>Date of reaching GWLs: CMIP5 (OEKS15) vs. CMIP5 (whole ensemble) vs. CMIP6</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
+        <cx:plotSurface>
+          <cx:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </cx:spPr>
+        </cx:plotSurface>
         <cx:series layoutId="boxWhisker" uniqueId="{00000007-8C2E-6046-9CB2-CB9C5341ECB9}" formatIdx="0">
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>1,5°C oeks</cx:v>
+              <cx:v>1.5°C OEKS15 (16)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3223,7 +3370,7 @@
           </cx:spPr>
           <cx:dataId val="0"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3231,7 +3378,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>1,5°C CMIP5</cx:v>
+              <cx:v>1.5°C CMIP5 (24)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3249,7 +3396,7 @@
           </cx:spPr>
           <cx:dataId val="1"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3257,7 +3404,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>1,5°C CMIP6</cx:v>
+              <cx:v>1.5°C CMIP6 (178)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3275,7 +3422,7 @@
           </cx:spPr>
           <cx:dataId val="2"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3289,7 +3436,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>2,0°C oeks</cx:v>
+              <cx:v>2.0°C OEKS15 (12)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3307,7 +3454,7 @@
           </cx:spPr>
           <cx:dataId val="4"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3315,7 +3462,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>2,0°C CMIP5</cx:v>
+              <cx:v>2.0°C CMIP5 (21)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3333,7 +3480,7 @@
           </cx:spPr>
           <cx:dataId val="5"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3341,7 +3488,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>2,0°C CMIP6</cx:v>
+              <cx:v>2.0°C CMIP6 (160)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3359,7 +3506,7 @@
           </cx:spPr>
           <cx:dataId val="6"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3373,7 +3520,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>3,0°C oeks</cx:v>
+              <cx:v>3.0°C OEKS15 (9)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3391,7 +3538,7 @@
           </cx:spPr>
           <cx:dataId val="8"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3399,7 +3546,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>3,0°C CMIP5</cx:v>
+              <cx:v>3.0°C CMIP5 (11)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3417,7 +3564,7 @@
           </cx:spPr>
           <cx:dataId val="9"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3425,7 +3572,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>3,0°C CMIP6</cx:v>
+              <cx:v>3.0°C CMIP6 (105)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3443,7 +3590,7 @@
           </cx:spPr>
           <cx:dataId val="10"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3457,7 +3604,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>4,0°C oeks</cx:v>
+              <cx:v>4.0°C OEKS15 (5)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3474,7 +3621,7 @@
           </cx:spPr>
           <cx:dataId val="12"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3482,7 +3629,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>4,0°C CMIP5</cx:v>
+              <cx:v>4.0°C CMIP5 (6)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3499,7 +3646,7 @@
           </cx:spPr>
           <cx:dataId val="13"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3507,7 +3654,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>4,0°C CMIP6</cx:v>
+              <cx:v>4.0°C CMIP6 (54)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3524,7 +3671,7 @@
           </cx:spPr>
           <cx:dataId val="14"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -3535,19 +3682,76 @@
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling min="2000"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Year</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1200"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Year</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
+        <cx:majorTickMarks type="out"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
     </cx:plotArea>
-    <cx:legend pos="r" align="ctr" overlay="0">
+    <cx:legend pos="r" align="ctr" overlay="1">
+      <cx:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="DADADA"/>
+          </a:solidFill>
+        </a:ln>
+      </cx:spPr>
       <cx:txPr>
         <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
+            <a:defRPr sz="1200"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:endParaRPr lang="de-DE" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000">
                 <a:lumMod val="65000"/>
@@ -3568,49 +3772,75 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.26</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.24</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.30</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.28</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Date of reaching GWLs for three RCPs within the CMIP5 ensemble</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1600" b="1"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Date of reaching GWLs for three RCPs within the CMIP5 ensemble</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:plotSurface>
           <cx:spPr>
             <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="DADADA"/>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
           </cx:spPr>
         </cx:plotSurface>
@@ -3618,7 +3848,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>1.5°C rcp2.6</cx:v>
+              <cx:v>1.5°C RCP 2.6 (8)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3644,7 +3874,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>1.5°C rcp4.5</cx:v>
+              <cx:v>1.5°C RCP 4.5 (8)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3670,7 +3900,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>1.5°C rcp8.5</cx:v>
+              <cx:v>1.5°C RCP 8.5 (8)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3701,7 +3931,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>2.0°C rcp2.6</cx:v>
+              <cx:v>2.0°C RCP 2.6 (5)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3727,7 +3957,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>2.0°C rcp4.5</cx:v>
+              <cx:v>2.0°C RCP 4.5 (8)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3753,7 +3983,7 @@
           <cx:tx>
             <cx:txData>
               <cx:f/>
-              <cx:v>2.0°C rcp8.5</cx:v>
+              <cx:v>2.0°C RCP 8.5 (8)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
@@ -3810,7 +4040,380 @@
           </cx:txPr>
         </cx:title>
         <cx:majorGridlines/>
+        <cx:majorTickMarks type="out"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="r" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+          </a:endParaRPr>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.31</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.35</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.32</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.36</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="4">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.33</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="5">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.37</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="6">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.34</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="7">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.38</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>Regional climate change signal (relative to 1991-2020) over Austria for four GWLs:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>CMIP5 vs. CMIP6</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{501E6A9F-23A5-0C49-8635-A0533F194E55}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>1.5°C CMIP5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000003-BC21-524E-A645-D6D07820167B}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>1.5°C CMIP6</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000004-BC21-524E-A645-D6D07820167B}" formatIdx="2">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>2.0°C CMIP5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000005-BC21-524E-A645-D6D07820167B}" formatIdx="3">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>2.0°C CMIP6</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000006-BC21-524E-A645-D6D07820167B}" formatIdx="4">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>3.0°C CMIP5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="4"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000007-BC21-524E-A645-D6D07820167B}" formatIdx="5">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>3.0°C CMIP6</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="5"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000008-BC21-524E-A645-D6D07820167B}" formatIdx="6">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>4.0°C CMIP5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="6"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000009-BC21-524E-A645-D6D07820167B}" formatIdx="7">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>4.0°C CMIP6</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="7"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Mean temperature change relative to 1991-2020 (°C)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1200"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Mean temperature change relative to 1991-2020 (°C)</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:minorGridlines/>
+        <cx:majorTickMarks type="out"/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="0" sourceLinked="0"/>
         <cx:txPr>
           <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
@@ -3831,7 +4434,17 @@
         </cx:txPr>
       </cx:axis>
     </cx:plotArea>
-    <cx:legend pos="r" align="ctr" overlay="0">
+    <cx:legend pos="r" align="ctr" overlay="1">
+      <cx:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="DADADA"/>
+          </a:solidFill>
+        </a:ln>
+      </cx:spPr>
       <cx:txPr>
         <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
@@ -3855,357 +4468,22 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="2">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.20</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="3">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.24</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="4">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="5">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="6">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.22</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="7">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.26</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0">
-      <cx:tx>
-        <cx:rich>
-          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr" rtl="0">
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              </a:rPr>
-              <a:t>Climate change signal AT (1991-2020) from GCM</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr" rtl="0">
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              </a:rPr>
-              <a:t>CMIP5 vs. CMIP6</a:t>
-            </a:r>
-          </a:p>
-        </cx:rich>
-      </cx:tx>
-    </cx:title>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{501E6A9F-23A5-0C49-8635-A0533F194E55}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f/>
-              <cx:v>1,5°C CMIP5</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{00000003-BC21-524E-A645-D6D07820167B}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f/>
-              <cx:v>1,5°C CMIP6</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{00000004-BC21-524E-A645-D6D07820167B}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f/>
-              <cx:v>2,0°C CMIP5</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="2"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{00000005-BC21-524E-A645-D6D07820167B}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f/>
-              <cx:v>2,0°C CMIP6</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="3"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{00000006-BC21-524E-A645-D6D07820167B}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f/>
-              <cx:v>3,0°C CMIP5</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="4"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{00000007-BC21-524E-A645-D6D07820167B}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f/>
-              <cx:v>3,0°C CMIP6</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="5"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{00000008-BC21-524E-A645-D6D07820167B}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f/>
-              <cx:v>4,0°C CMIP5</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="6"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="1" nonoutliers="0"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{00000009-BC21-524E-A645-D6D07820167B}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f/>
-              <cx:v>4,0°C CMIP6</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:spPr>
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:ln>
-          </cx:spPr>
-          <cx:dataId val="7"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0" hidden="1">
-        <cx:catScaling gapWidth="1"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:title>
-          <cx:tx>
-            <cx:txData>
-              <cx:v>Temperature change relative to 1991-2020</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:txPr>
-            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="de-DE" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:sysClr>
-                  </a:solidFill>
-                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                </a:rPr>
-                <a:t>Temperature change relative to 1991-2020</a:t>
-              </a:r>
-            </a:p>
-          </cx:txPr>
-        </cx:title>
-        <cx:majorGridlines/>
-        <cx:minorGridlines/>
-        <cx:minorTickMarks type="out"/>
-        <cx:tickLabels/>
-        <cx:numFmt formatCode="#.##0,0" sourceLinked="0"/>
-      </cx:axis>
-    </cx:plotArea>
-    <cx:legend pos="r" align="ctr" overlay="0"/>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
 <file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.36</cx:f>
+        <cx:f>_xlchart.v1.44</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.38</cx:f>
+        <cx:f>_xlchart.v1.46</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.40</cx:f>
+        <cx:f>_xlchart.v1.48</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4276,7 +4554,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24BF4607-F4E8-E345-97F3-975C8A945A06}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.35</cx:f>
+              <cx:f>_xlchart.v1.43</cx:f>
               <cx:v>rcp26</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4289,7 +4567,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B15400F1-0218-BE43-9F95-AD4EAABB47CD}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.37</cx:f>
+              <cx:f>_xlchart.v1.45</cx:f>
               <cx:v>rcp45</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4302,7 +4580,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{99A6A248-8D06-4B4A-861B-9E311114F9A0}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.39</cx:f>
+              <cx:f>_xlchart.v1.47</cx:f>
               <cx:v>rcp85</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4368,22 +4646,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.41</cx:f>
+        <cx:f>_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.42</cx:f>
+        <cx:f>_xlchart.v1.40</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.43</cx:f>
+        <cx:f>_xlchart.v1.41</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.44</cx:f>
+        <cx:f>_xlchart.v1.42</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8523,7 +8801,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B69F82F6-F9ED-9A4B-8D7B-52970A2F5AC9}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="185" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="126" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8545,7 +8823,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BE674C58-D2A4-B440-B0FB-F7B77C5D9F8F}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="185" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="136" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8600,7 +8878,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9315622" cy="6027351"/>
+    <xdr:ext cx="9313333" cy="6017381"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
@@ -8666,7 +8944,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{318E6868-8130-118B-A1D7-A96E632B99EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8086AF9-A943-6133-67F5-574DEE72765C}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -8677,7 +8955,7 @@
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="0"/>
-          <a:ext cx="9315622" cy="6027351"/>
+          <a:ext cx="9313333" cy="6017381"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -8777,7 +9055,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D515273-EE15-C455-5F45-AC20FC867064}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A23F10C9-FCE6-789C-FC98-ABB9FC287EB4}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -8822,7 +9100,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9315622" cy="6027351"/>
+    <xdr:ext cx="9319559" cy="6032500"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
@@ -8888,7 +9166,7 @@
         <cdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C463DE76-C613-AE6A-0441-1161334F9CC4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D8BE45E-B47A-A273-0569-D63809A05DCF}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -8899,7 +9177,7 @@
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="0" y="0"/>
-          <a:ext cx="9315622" cy="6027351"/>
+          <a:ext cx="9319559" cy="6032500"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -9611,12 +9889,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3"/>
-          <cell r="K3"/>
-          <cell r="L3"/>
-          <cell r="M3"/>
-        </row>
         <row r="4">
           <cell r="B4">
             <v>2068</v>
@@ -9624,9 +9896,6 @@
           <cell r="J4">
             <v>0.953297643723377</v>
           </cell>
-          <cell r="K4"/>
-          <cell r="L4"/>
-          <cell r="M4"/>
         </row>
         <row r="5">
           <cell r="B5">
@@ -9641,8 +9910,6 @@
           <cell r="K5">
             <v>1.12528774120191</v>
           </cell>
-          <cell r="L5"/>
-          <cell r="M5"/>
         </row>
         <row r="6">
           <cell r="B6">
@@ -9651,9 +9918,6 @@
           <cell r="J6">
             <v>0.962655414052216</v>
           </cell>
-          <cell r="K6"/>
-          <cell r="L6"/>
-          <cell r="M6"/>
         </row>
         <row r="7">
           <cell r="B7">
@@ -9668,20 +9932,6 @@
           <cell r="K7">
             <v>0.75275346345142902</v>
           </cell>
-          <cell r="L7"/>
-          <cell r="M7"/>
-        </row>
-        <row r="8">
-          <cell r="J8"/>
-          <cell r="K8"/>
-          <cell r="L8"/>
-          <cell r="M8"/>
-        </row>
-        <row r="9">
-          <cell r="J9"/>
-          <cell r="K9"/>
-          <cell r="L9"/>
-          <cell r="M9"/>
         </row>
         <row r="10">
           <cell r="B10">
@@ -9696,26 +9946,6 @@
           <cell r="K10">
             <v>1.2996490999999999</v>
           </cell>
-          <cell r="L10"/>
-          <cell r="M10"/>
-        </row>
-        <row r="11">
-          <cell r="J11"/>
-          <cell r="K11"/>
-          <cell r="L11"/>
-          <cell r="M11"/>
-        </row>
-        <row r="12">
-          <cell r="J12"/>
-          <cell r="K12"/>
-          <cell r="L12"/>
-          <cell r="M12"/>
-        </row>
-        <row r="13">
-          <cell r="J13"/>
-          <cell r="K13"/>
-          <cell r="L13"/>
-          <cell r="M13"/>
         </row>
         <row r="14">
           <cell r="B14">
@@ -9724,9 +9954,6 @@
           <cell r="J14">
             <v>1.1676970687033701</v>
           </cell>
-          <cell r="K14"/>
-          <cell r="L14"/>
-          <cell r="M14"/>
         </row>
         <row r="15">
           <cell r="B15">
@@ -9741,8 +9968,6 @@
           <cell r="K15">
             <v>2.1459751510413598</v>
           </cell>
-          <cell r="L15"/>
-          <cell r="M15"/>
         </row>
         <row r="16">
           <cell r="B16">
@@ -9757,8 +9982,6 @@
           <cell r="K16">
             <v>1.8127139886377099</v>
           </cell>
-          <cell r="L16"/>
-          <cell r="M16"/>
         </row>
         <row r="17">
           <cell r="B17">
@@ -9773,8 +9996,6 @@
           <cell r="K17">
             <v>1.8433555303092599</v>
           </cell>
-          <cell r="L17"/>
-          <cell r="M17"/>
         </row>
         <row r="18">
           <cell r="B18">
@@ -9789,8 +10010,6 @@
           <cell r="K18">
             <v>1.2746751758441699</v>
           </cell>
-          <cell r="L18"/>
-          <cell r="M18"/>
         </row>
         <row r="19">
           <cell r="B19">
@@ -9799,15 +10018,6 @@
           <cell r="J19">
             <v>0.50765736677745898</v>
           </cell>
-          <cell r="K19"/>
-          <cell r="L19"/>
-          <cell r="M19"/>
-        </row>
-        <row r="20">
-          <cell r="J20"/>
-          <cell r="K20"/>
-          <cell r="L20"/>
-          <cell r="M20"/>
         </row>
         <row r="21">
           <cell r="B21">
@@ -9822,8 +10032,6 @@
           <cell r="K21">
             <v>3.1213066025999701</v>
           </cell>
-          <cell r="L21"/>
-          <cell r="M21"/>
         </row>
         <row r="22">
           <cell r="B22">
@@ -9838,8 +10046,6 @@
           <cell r="K22">
             <v>1.3981454217936999</v>
           </cell>
-          <cell r="L22"/>
-          <cell r="M22"/>
         </row>
         <row r="23">
           <cell r="B23">
@@ -9854,8 +10060,6 @@
           <cell r="K23">
             <v>1.67016129100406</v>
           </cell>
-          <cell r="L23"/>
-          <cell r="M23"/>
         </row>
         <row r="24">
           <cell r="B24">
@@ -9870,8 +10074,6 @@
           <cell r="K24">
             <v>1.0728179942746401</v>
           </cell>
-          <cell r="L24"/>
-          <cell r="M24"/>
         </row>
         <row r="25">
           <cell r="B25">
@@ -9886,8 +10088,6 @@
           <cell r="K25">
             <v>1.6734034587411499</v>
           </cell>
-          <cell r="L25"/>
-          <cell r="M25"/>
         </row>
         <row r="26">
           <cell r="B26">
@@ -9902,8 +10102,6 @@
           <cell r="K26">
             <v>0.94311847540844496</v>
           </cell>
-          <cell r="L26"/>
-          <cell r="M26"/>
         </row>
         <row r="27">
           <cell r="B27">
@@ -9918,8 +10116,6 @@
           <cell r="K27">
             <v>1.4934826904101901</v>
           </cell>
-          <cell r="L27"/>
-          <cell r="M27"/>
         </row>
         <row r="28">
           <cell r="B28">
@@ -9928,9 +10124,6 @@
           <cell r="J28">
             <v>1.0283560461610499</v>
           </cell>
-          <cell r="K28"/>
-          <cell r="L28"/>
-          <cell r="M28"/>
         </row>
         <row r="29">
           <cell r="B29">
@@ -9945,8 +10138,6 @@
           <cell r="K29">
             <v>0.45363177546752198</v>
           </cell>
-          <cell r="L29"/>
-          <cell r="M29"/>
         </row>
         <row r="30">
           <cell r="B30">
@@ -9961,8 +10152,6 @@
           <cell r="K30">
             <v>0.91811225325973</v>
           </cell>
-          <cell r="L30"/>
-          <cell r="M30"/>
         </row>
         <row r="31">
           <cell r="B31">
@@ -9971,9 +10160,6 @@
           <cell r="J31">
             <v>1.0129333473675</v>
           </cell>
-          <cell r="K31"/>
-          <cell r="L31"/>
-          <cell r="M31"/>
         </row>
         <row r="32">
           <cell r="B32">
@@ -9988,8 +10174,6 @@
           <cell r="K32">
             <v>0.93398420658576498</v>
           </cell>
-          <cell r="L32"/>
-          <cell r="M32"/>
         </row>
         <row r="33">
           <cell r="B33">
@@ -10004,8 +10188,6 @@
           <cell r="K33">
             <v>1.9070619275280301</v>
           </cell>
-          <cell r="L33"/>
-          <cell r="M33"/>
         </row>
         <row r="34">
           <cell r="B34">
@@ -10020,14 +10202,6 @@
           <cell r="K34">
             <v>1.03584774279575</v>
           </cell>
-          <cell r="L34"/>
-          <cell r="M34"/>
-        </row>
-        <row r="35">
-          <cell r="J35"/>
-          <cell r="K35"/>
-          <cell r="L35"/>
-          <cell r="M35"/>
         </row>
         <row r="36">
           <cell r="B36">
@@ -10042,14 +10216,6 @@
           <cell r="K36">
             <v>1.1211079653474301</v>
           </cell>
-          <cell r="L36"/>
-          <cell r="M36"/>
-        </row>
-        <row r="37">
-          <cell r="J37"/>
-          <cell r="K37"/>
-          <cell r="L37"/>
-          <cell r="M37"/>
         </row>
         <row r="38">
           <cell r="B38">
@@ -10058,9 +10224,6 @@
           <cell r="J38">
             <v>1.47924744842162</v>
           </cell>
-          <cell r="K38"/>
-          <cell r="L38"/>
-          <cell r="M38"/>
         </row>
         <row r="39">
           <cell r="B39">
@@ -10075,8 +10238,6 @@
           <cell r="K39">
             <v>1.47625627991256</v>
           </cell>
-          <cell r="L39"/>
-          <cell r="M39"/>
         </row>
         <row r="40">
           <cell r="B40">
@@ -10091,8 +10252,6 @@
           <cell r="K40">
             <v>1.22094780806839</v>
           </cell>
-          <cell r="L40"/>
-          <cell r="M40"/>
         </row>
         <row r="41">
           <cell r="B41">
@@ -10107,8 +10266,6 @@
           <cell r="K41">
             <v>1.7052057166927399</v>
           </cell>
-          <cell r="L41"/>
-          <cell r="M41"/>
         </row>
         <row r="42">
           <cell r="B42">
@@ -10117,9 +10274,6 @@
           <cell r="J42">
             <v>0.81285915249012197</v>
           </cell>
-          <cell r="K42"/>
-          <cell r="L42"/>
-          <cell r="M42"/>
         </row>
         <row r="43">
           <cell r="B43">
@@ -10128,9 +10282,6 @@
           <cell r="J43">
             <v>0.85479150373844803</v>
           </cell>
-          <cell r="K43"/>
-          <cell r="L43"/>
-          <cell r="M43"/>
         </row>
         <row r="44">
           <cell r="B44">
@@ -10139,9 +10290,6 @@
           <cell r="J44">
             <v>1.24668562684192</v>
           </cell>
-          <cell r="K44"/>
-          <cell r="L44"/>
-          <cell r="M44"/>
         </row>
         <row r="45">
           <cell r="B45">
@@ -10182,8 +10330,6 @@
           <cell r="K46">
             <v>0.99413149999999995</v>
           </cell>
-          <cell r="L46"/>
-          <cell r="M46"/>
         </row>
         <row r="47">
           <cell r="B47">
@@ -10198,8 +10344,6 @@
           <cell r="K47">
             <v>1.2139563001517599</v>
           </cell>
-          <cell r="L47"/>
-          <cell r="M47"/>
         </row>
         <row r="48">
           <cell r="B48">
@@ -10208,9 +10352,6 @@
           <cell r="J48">
             <v>0.31548891067506302</v>
           </cell>
-          <cell r="K48"/>
-          <cell r="L48"/>
-          <cell r="M48"/>
         </row>
         <row r="49">
           <cell r="B49">
@@ -10225,8 +10366,6 @@
           <cell r="K49">
             <v>1.43005460103351</v>
           </cell>
-          <cell r="L49"/>
-          <cell r="M49"/>
         </row>
         <row r="50">
           <cell r="B50">
@@ -10235,9 +10374,6 @@
           <cell r="J50">
             <v>1.58398556179473</v>
           </cell>
-          <cell r="K50"/>
-          <cell r="L50"/>
-          <cell r="M50"/>
         </row>
         <row r="51">
           <cell r="B51">
@@ -10246,9 +10382,6 @@
           <cell r="J51">
             <v>1.5601286800869001</v>
           </cell>
-          <cell r="K51"/>
-          <cell r="L51"/>
-          <cell r="M51"/>
         </row>
         <row r="52">
           <cell r="B52">
@@ -10257,9 +10390,6 @@
           <cell r="J52">
             <v>0.89465247498328804</v>
           </cell>
-          <cell r="K52"/>
-          <cell r="L52"/>
-          <cell r="M52"/>
         </row>
         <row r="53">
           <cell r="B53">
@@ -10268,9 +10398,6 @@
           <cell r="J53">
             <v>1.4470739576551801</v>
           </cell>
-          <cell r="K53"/>
-          <cell r="L53"/>
-          <cell r="M53"/>
         </row>
         <row r="54">
           <cell r="B54">
@@ -10279,9 +10406,6 @@
           <cell r="J54">
             <v>0.93532776547523599</v>
           </cell>
-          <cell r="K54"/>
-          <cell r="L54"/>
-          <cell r="M54"/>
         </row>
         <row r="55">
           <cell r="B55">
@@ -10296,20 +10420,6 @@
           <cell r="K55">
             <v>1.4829433865017501</v>
           </cell>
-          <cell r="L55"/>
-          <cell r="M55"/>
-        </row>
-        <row r="56">
-          <cell r="J56"/>
-          <cell r="K56"/>
-          <cell r="L56"/>
-          <cell r="M56"/>
-        </row>
-        <row r="57">
-          <cell r="J57"/>
-          <cell r="K57"/>
-          <cell r="L57"/>
-          <cell r="M57"/>
         </row>
         <row r="58">
           <cell r="B58">
@@ -10324,8 +10434,6 @@
           <cell r="K58">
             <v>1.7895930232263599</v>
           </cell>
-          <cell r="L58"/>
-          <cell r="M58"/>
         </row>
         <row r="59">
           <cell r="B59">
@@ -10340,8 +10448,6 @@
           <cell r="K59">
             <v>1.8116578232415801</v>
           </cell>
-          <cell r="L59"/>
-          <cell r="M59"/>
         </row>
         <row r="60">
           <cell r="B60">
@@ -10362,7 +10468,6 @@
           <cell r="L60">
             <v>3.0059425348697002</v>
           </cell>
-          <cell r="M60"/>
         </row>
         <row r="61">
           <cell r="B61">
@@ -10377,8 +10482,6 @@
           <cell r="K61">
             <v>1.7521867119608101</v>
           </cell>
-          <cell r="L61"/>
-          <cell r="M61"/>
         </row>
         <row r="62">
           <cell r="B62">
@@ -10393,8 +10496,6 @@
           <cell r="K62">
             <v>1.1976161575342901</v>
           </cell>
-          <cell r="L62"/>
-          <cell r="M62"/>
         </row>
         <row r="63">
           <cell r="B63">
@@ -10409,8 +10510,6 @@
           <cell r="K63">
             <v>1.79025508687392</v>
           </cell>
-          <cell r="L63"/>
-          <cell r="M63"/>
         </row>
         <row r="64">
           <cell r="B64">
@@ -10425,8 +10524,6 @@
           <cell r="K64">
             <v>1.8836058328781899</v>
           </cell>
-          <cell r="L64"/>
-          <cell r="M64"/>
         </row>
         <row r="65">
           <cell r="B65">
@@ -10447,7 +10544,6 @@
           <cell r="L65">
             <v>4.2916051539023199</v>
           </cell>
-          <cell r="M65"/>
         </row>
         <row r="66">
           <cell r="B66">
@@ -10468,7 +10564,6 @@
           <cell r="L66">
             <v>2.0659365442925499</v>
           </cell>
-          <cell r="M66"/>
         </row>
         <row r="67">
           <cell r="B67">
@@ -10489,7 +10584,6 @@
           <cell r="L67">
             <v>2.07600407171268</v>
           </cell>
-          <cell r="M67"/>
         </row>
         <row r="68">
           <cell r="B68">
@@ -10510,7 +10604,6 @@
           <cell r="L68">
             <v>2.46145115976516</v>
           </cell>
-          <cell r="M68"/>
         </row>
         <row r="69">
           <cell r="B69">
@@ -10531,7 +10624,6 @@
           <cell r="L69">
             <v>2.95128872598479</v>
           </cell>
-          <cell r="M69"/>
         </row>
         <row r="70">
           <cell r="B70">
@@ -10552,7 +10644,6 @@
           <cell r="L70">
             <v>2.4659900553596299</v>
           </cell>
-          <cell r="M70"/>
         </row>
         <row r="71">
           <cell r="B71">
@@ -10573,7 +10664,6 @@
           <cell r="L71">
             <v>1.9276448337221399</v>
           </cell>
-          <cell r="M71"/>
         </row>
         <row r="72">
           <cell r="B72">
@@ -10594,7 +10684,6 @@
           <cell r="L72">
             <v>2.2183875868211</v>
           </cell>
-          <cell r="M72"/>
         </row>
         <row r="73">
           <cell r="B73">
@@ -10667,7 +10756,6 @@
           <cell r="L75">
             <v>1.7990900046379901</v>
           </cell>
-          <cell r="M75"/>
         </row>
         <row r="76">
           <cell r="B76">
@@ -10688,7 +10776,6 @@
           <cell r="L76">
             <v>2.3771028757036698</v>
           </cell>
-          <cell r="M76"/>
         </row>
         <row r="77">
           <cell r="B77">
@@ -10709,7 +10796,6 @@
           <cell r="L77">
             <v>1.64459827038435</v>
           </cell>
-          <cell r="M77"/>
         </row>
         <row r="78">
           <cell r="B78">
@@ -10730,7 +10816,6 @@
           <cell r="L78">
             <v>2.4737583558019298</v>
           </cell>
-          <cell r="M78"/>
         </row>
         <row r="79">
           <cell r="B79">
@@ -10745,8 +10830,6 @@
           <cell r="K79">
             <v>1.1256945521228801</v>
           </cell>
-          <cell r="L79"/>
-          <cell r="M79"/>
         </row>
         <row r="80">
           <cell r="B80">
@@ -10761,8 +10844,6 @@
           <cell r="K80">
             <v>1.42677008310954</v>
           </cell>
-          <cell r="L80"/>
-          <cell r="M80"/>
         </row>
         <row r="81">
           <cell r="B81">
@@ -10783,7 +10864,6 @@
           <cell r="L81">
             <v>2.1591106380818599</v>
           </cell>
-          <cell r="M81"/>
         </row>
         <row r="82">
           <cell r="B82">
@@ -10798,8 +10878,6 @@
           <cell r="K82">
             <v>1.6772889300680101</v>
           </cell>
-          <cell r="L82"/>
-          <cell r="M82"/>
         </row>
         <row r="83">
           <cell r="B83">
@@ -10814,8 +10892,6 @@
           <cell r="K83">
             <v>1.65557634817044</v>
           </cell>
-          <cell r="L83"/>
-          <cell r="M83"/>
         </row>
         <row r="84">
           <cell r="B84">
@@ -10830,8 +10906,6 @@
           <cell r="K84">
             <v>1.79784619645486</v>
           </cell>
-          <cell r="L84"/>
-          <cell r="M84"/>
         </row>
         <row r="85">
           <cell r="B85">
@@ -10846,8 +10920,6 @@
           <cell r="K85">
             <v>1.7099448768059999</v>
           </cell>
-          <cell r="L85"/>
-          <cell r="M85"/>
         </row>
         <row r="86">
           <cell r="B86">
@@ -10868,7 +10940,6 @@
           <cell r="L86">
             <v>2.7137934503127701</v>
           </cell>
-          <cell r="M86"/>
         </row>
         <row r="87">
           <cell r="B87">
@@ -10889,7 +10960,6 @@
           <cell r="L87">
             <v>2.6473017385885602</v>
           </cell>
-          <cell r="M87"/>
         </row>
         <row r="88">
           <cell r="B88">
@@ -10904,8 +10974,6 @@
           <cell r="K88">
             <v>1.4064785184664499</v>
           </cell>
-          <cell r="L88"/>
-          <cell r="M88"/>
         </row>
         <row r="89">
           <cell r="B89">
@@ -10920,8 +10988,6 @@
           <cell r="K89">
             <v>1.8829193396530901</v>
           </cell>
-          <cell r="L89"/>
-          <cell r="M89"/>
         </row>
         <row r="90">
           <cell r="B90">
@@ -10936,8 +11002,6 @@
           <cell r="K90">
             <v>1.9885308508852599</v>
           </cell>
-          <cell r="L90"/>
-          <cell r="M90"/>
         </row>
         <row r="91">
           <cell r="B91">
@@ -10958,7 +11022,6 @@
           <cell r="L91">
             <v>2.7629134999999998</v>
           </cell>
-          <cell r="M91"/>
         </row>
         <row r="92">
           <cell r="B92">
@@ -10979,7 +11042,6 @@
           <cell r="L92">
             <v>2.61799366766664</v>
           </cell>
-          <cell r="M92"/>
         </row>
         <row r="93">
           <cell r="B93">
@@ -10994,8 +11056,6 @@
           <cell r="K93">
             <v>0.74702986611260902</v>
           </cell>
-          <cell r="L93"/>
-          <cell r="M93"/>
         </row>
         <row r="94">
           <cell r="B94">
@@ -11010,8 +11070,6 @@
           <cell r="K94">
             <v>1.81199906667073</v>
           </cell>
-          <cell r="L94"/>
-          <cell r="M94"/>
         </row>
         <row r="95">
           <cell r="B95">
@@ -11026,8 +11084,6 @@
           <cell r="K95">
             <v>2.3510983361137998</v>
           </cell>
-          <cell r="L95"/>
-          <cell r="M95"/>
         </row>
         <row r="96">
           <cell r="B96">
@@ -11042,8 +11098,6 @@
           <cell r="K96">
             <v>1.8110792384853101</v>
           </cell>
-          <cell r="L96"/>
-          <cell r="M96"/>
         </row>
         <row r="97">
           <cell r="B97">
@@ -11058,8 +11112,6 @@
           <cell r="K97">
             <v>1.5849269976389799</v>
           </cell>
-          <cell r="L97"/>
-          <cell r="M97"/>
         </row>
         <row r="98">
           <cell r="B98">
@@ -11074,8 +11126,6 @@
           <cell r="K98">
             <v>1.61900668674048</v>
           </cell>
-          <cell r="L98"/>
-          <cell r="M98"/>
         </row>
         <row r="99">
           <cell r="B99">
@@ -11090,8 +11140,6 @@
           <cell r="K99">
             <v>1.3695843568142401</v>
           </cell>
-          <cell r="L99"/>
-          <cell r="M99"/>
         </row>
         <row r="100">
           <cell r="B100">
@@ -11106,8 +11154,6 @@
           <cell r="K100">
             <v>1.71808351940573</v>
           </cell>
-          <cell r="L100"/>
-          <cell r="M100"/>
         </row>
         <row r="101">
           <cell r="B101">
@@ -11122,8 +11168,6 @@
           <cell r="K101">
             <v>2.1603128362584698</v>
           </cell>
-          <cell r="L101"/>
-          <cell r="M101"/>
         </row>
         <row r="102">
           <cell r="B102">
@@ -11138,8 +11182,6 @@
           <cell r="K102">
             <v>1.9302608195684401</v>
           </cell>
-          <cell r="L102"/>
-          <cell r="M102"/>
         </row>
         <row r="103">
           <cell r="B103">
@@ -11160,7 +11202,6 @@
           <cell r="L103">
             <v>3.1708323798723201</v>
           </cell>
-          <cell r="M103"/>
         </row>
         <row r="104">
           <cell r="B104">
@@ -11233,7 +11274,6 @@
           <cell r="L106">
             <v>3.02139535831243</v>
           </cell>
-          <cell r="M106"/>
         </row>
         <row r="107">
           <cell r="B107">
@@ -11254,7 +11294,6 @@
           <cell r="L107">
             <v>2.7878231845461698</v>
           </cell>
-          <cell r="M107"/>
         </row>
         <row r="108">
           <cell r="B108">
@@ -11275,7 +11314,6 @@
           <cell r="L108">
             <v>3.1576496725510599</v>
           </cell>
-          <cell r="M108"/>
         </row>
         <row r="109">
           <cell r="B109">
@@ -11284,9 +11322,6 @@
           <cell r="J109">
             <v>1.5657428882740401</v>
           </cell>
-          <cell r="K109"/>
-          <cell r="L109"/>
-          <cell r="M109"/>
         </row>
         <row r="110">
           <cell r="B110">
@@ -11301,8 +11336,6 @@
           <cell r="K110">
             <v>1.8104741339919299</v>
           </cell>
-          <cell r="L110"/>
-          <cell r="M110"/>
         </row>
         <row r="111">
           <cell r="B111">
@@ -11323,7 +11356,6 @@
           <cell r="L111">
             <v>4.1255501015432303</v>
           </cell>
-          <cell r="M111"/>
         </row>
         <row r="112">
           <cell r="B112">
@@ -11682,7 +11714,6 @@
           <cell r="L125">
             <v>2.1705614599349499</v>
           </cell>
-          <cell r="M125"/>
         </row>
         <row r="126">
           <cell r="B126">
@@ -11703,7 +11734,6 @@
           <cell r="L126">
             <v>2.21875868903268</v>
           </cell>
-          <cell r="M126"/>
         </row>
         <row r="127">
           <cell r="B127">
@@ -11724,7 +11754,6 @@
           <cell r="L127">
             <v>3.0087400281739001</v>
           </cell>
-          <cell r="M127"/>
         </row>
         <row r="128">
           <cell r="B128">
@@ -11745,7 +11774,6 @@
           <cell r="L128">
             <v>2.5273760401932899</v>
           </cell>
-          <cell r="M128"/>
         </row>
         <row r="129">
           <cell r="B129">
@@ -11766,7 +11794,6 @@
           <cell r="L129">
             <v>2.6335885440636302</v>
           </cell>
-          <cell r="M129"/>
         </row>
         <row r="130">
           <cell r="B130">
@@ -11787,7 +11814,6 @@
           <cell r="L130">
             <v>2.3055320339923799</v>
           </cell>
-          <cell r="M130"/>
         </row>
         <row r="131">
           <cell r="B131">
@@ -11808,7 +11834,6 @@
           <cell r="L131">
             <v>2.8297057592542201</v>
           </cell>
-          <cell r="M131"/>
         </row>
         <row r="132">
           <cell r="B132">
@@ -11829,7 +11854,6 @@
           <cell r="L132">
             <v>3.20905435545248</v>
           </cell>
-          <cell r="M132"/>
         </row>
         <row r="133">
           <cell r="B133">
@@ -11928,7 +11952,6 @@
           <cell r="L136">
             <v>2.4212512758043401</v>
           </cell>
-          <cell r="M136"/>
         </row>
         <row r="137">
           <cell r="B137">
@@ -11949,7 +11972,6 @@
           <cell r="L137">
             <v>3.4698040573684898</v>
           </cell>
-          <cell r="M137"/>
         </row>
         <row r="138">
           <cell r="B138">
@@ -11964,8 +11986,6 @@
           <cell r="K138">
             <v>2.2215974851091702</v>
           </cell>
-          <cell r="L138"/>
-          <cell r="M138"/>
         </row>
         <row r="139">
           <cell r="B139">
@@ -11974,9 +11994,6 @@
           <cell r="J139">
             <v>1.4871546851264099</v>
           </cell>
-          <cell r="K139"/>
-          <cell r="L139"/>
-          <cell r="M139"/>
         </row>
         <row r="140">
           <cell r="B140">
@@ -11997,7 +12014,6 @@
           <cell r="L140">
             <v>2.76461721959198</v>
           </cell>
-          <cell r="M140"/>
         </row>
         <row r="141">
           <cell r="B141">
@@ -12018,7 +12034,6 @@
           <cell r="L141">
             <v>3.0094896104601001</v>
           </cell>
-          <cell r="M141"/>
         </row>
         <row r="142">
           <cell r="B142">
@@ -12039,7 +12054,6 @@
           <cell r="L142">
             <v>2.2740586286362601</v>
           </cell>
-          <cell r="M142"/>
         </row>
         <row r="143">
           <cell r="B143">
@@ -12054,8 +12068,6 @@
           <cell r="K143">
             <v>2.1390993330213699</v>
           </cell>
-          <cell r="L143"/>
-          <cell r="M143"/>
         </row>
         <row r="144">
           <cell r="B144">
@@ -12076,7 +12088,6 @@
           <cell r="L144">
             <v>3.6687247613706999</v>
           </cell>
-          <cell r="M144"/>
         </row>
         <row r="145">
           <cell r="B145">
@@ -12227,7 +12238,6 @@
           <cell r="L150">
             <v>3.30951525175441</v>
           </cell>
-          <cell r="M150"/>
         </row>
         <row r="151">
           <cell r="B151">
@@ -12248,7 +12258,6 @@
           <cell r="L151">
             <v>2.9504145044591001</v>
           </cell>
-          <cell r="M151"/>
         </row>
         <row r="152">
           <cell r="B152">
@@ -12659,7 +12668,6 @@
           <cell r="L167">
             <v>2.2516428417629699</v>
           </cell>
-          <cell r="M167"/>
         </row>
         <row r="168">
           <cell r="B168">
@@ -12758,7 +12766,6 @@
           <cell r="L171">
             <v>3.04848111038363</v>
           </cell>
-          <cell r="M171"/>
         </row>
         <row r="172">
           <cell r="B172">
@@ -12857,7 +12864,6 @@
           <cell r="L175">
             <v>2.5286943670620601</v>
           </cell>
-          <cell r="M175"/>
         </row>
         <row r="176">
           <cell r="B176">
@@ -12878,7 +12884,6 @@
           <cell r="L176">
             <v>2.7677175902520599</v>
           </cell>
-          <cell r="M176"/>
         </row>
         <row r="177">
           <cell r="B177">
@@ -12899,7 +12904,6 @@
           <cell r="L177">
             <v>2.9216101985538199</v>
           </cell>
-          <cell r="M177"/>
         </row>
         <row r="178">
           <cell r="B178">
@@ -12972,7 +12976,6 @@
           <cell r="L180">
             <v>2.3987316555447</v>
           </cell>
-          <cell r="M180"/>
         </row>
         <row r="181">
           <cell r="B181">
@@ -13019,7 +13022,6 @@
           <cell r="L182">
             <v>3.49936630814164</v>
           </cell>
-          <cell r="M182"/>
         </row>
         <row r="183">
           <cell r="B183">
@@ -13040,7 +13042,6 @@
           <cell r="L183">
             <v>3.3262258100273101</v>
           </cell>
-          <cell r="M183"/>
         </row>
         <row r="184">
           <cell r="B184">
@@ -13061,7 +13062,6 @@
           <cell r="L184">
             <v>2.8145093766053302</v>
           </cell>
-          <cell r="M184"/>
         </row>
         <row r="185">
           <cell r="B185">
@@ -13082,7 +13082,6 @@
           <cell r="L185">
             <v>2.8472741021049801</v>
           </cell>
-          <cell r="M185"/>
         </row>
         <row r="186">
           <cell r="B186">
@@ -13155,7 +13154,6 @@
           <cell r="L188">
             <v>3.3017069074842902</v>
           </cell>
-          <cell r="M188"/>
         </row>
         <row r="189">
           <cell r="B189">
@@ -13176,7 +13174,6 @@
           <cell r="L189">
             <v>3.3375443506061302</v>
           </cell>
-          <cell r="M189"/>
         </row>
         <row r="190">
           <cell r="B190">
@@ -13536,7 +13533,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14009,8 +14006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8388F6E0-5660-DB40-B6C7-A98F3137AF83}">
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14024,34 +14021,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -14110,7 +14107,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
@@ -14136,7 +14133,7 @@
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
@@ -14162,7 +14159,7 @@
       <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
@@ -14188,7 +14185,7 @@
       <c r="R5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
@@ -14214,7 +14211,7 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
@@ -14240,7 +14237,7 @@
       <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
@@ -14266,7 +14263,7 @@
       <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
@@ -14292,7 +14289,7 @@
       <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
@@ -14328,7 +14325,7 @@
       <c r="R10" s="3"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
@@ -14364,7 +14361,7 @@
       <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
@@ -14400,7 +14397,7 @@
       <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
@@ -14436,7 +14433,7 @@
       <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
@@ -14472,7 +14469,7 @@
       <c r="R14" s="3"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
@@ -14508,7 +14505,7 @@
       <c r="R15" s="3"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B16" t="s">
@@ -14554,7 +14551,7 @@
       <c r="R16" s="3"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
@@ -14600,7 +14597,7 @@
       <c r="R17" s="3"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B18" t="s">
@@ -14646,7 +14643,7 @@
       <c r="R18" s="3"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B19" t="s">
@@ -14692,7 +14689,7 @@
       <c r="R19" s="3"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="18" t="s">
         <v>46</v>
       </c>
       <c r="B20" t="s">
@@ -14728,7 +14725,7 @@
       <c r="R20" s="3"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="18" t="s">
         <v>46</v>
       </c>
       <c r="B21" t="s">
@@ -14764,7 +14761,7 @@
       <c r="R21" s="3"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B22" t="s">
@@ -14821,7 +14818,7 @@
       <c r="W22" s="3"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B23" t="s">
@@ -14878,7 +14875,7 @@
       <c r="W23" s="3"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B24" t="s">
@@ -14934,7 +14931,7 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B25" t="s">
@@ -14981,7 +14978,7 @@
       <c r="W25" s="3"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B26" t="s">
@@ -15027,7 +15024,7 @@
       <c r="R26" s="3"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="20" t="s">
         <v>63</v>
       </c>
       <c r="B27" t="s">
@@ -15083,7 +15080,7 @@
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B28" t="s">
@@ -15139,7 +15136,7 @@
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B29" t="s">
@@ -15195,7 +15192,7 @@
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="21" t="s">
         <v>74</v>
       </c>
       <c r="B30" t="s">
@@ -15251,7 +15248,7 @@
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="21" t="s">
         <v>74</v>
       </c>
       <c r="B31" t="s">
@@ -15307,7 +15304,7 @@
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B32" t="s">
@@ -15363,7 +15360,7 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B33" t="s">
@@ -15419,46 +15416,46 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="26"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="9" t="s">
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="9" t="s">
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="12" t="s">
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="R36" s="12"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
@@ -15688,13 +15685,13 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">

</xml_diff>